<commit_message>
modify minimization fitting Jupyter notebook to include all min code
</commit_message>
<xml_diff>
--- a/basinhop_TEMPLATE.xlsx
+++ b/basinhop_TEMPLATE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\garci\dropbox (personal)\scripts\statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4700ADB8-8617-4AA6-B64E-587C40D00B2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD584443-5150-4A07-9E6E-9D8FACABB750}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1882" yWindow="293" windowWidth="14401" windowHeight="6449" activeTab="1" xr2:uid="{BA8947B8-D0E5-4727-98DD-7F83DB71C123}"/>
   </bookViews>
@@ -1868,15 +1868,15 @@
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <f t="shared" ref="A2:B21" ca="1" si="0">_xlfn.NORM.INV(RAND(),0,0.5)</f>
-        <v>0.29057781274293554</v>
+        <v>1.0900626241572196</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.22624054426531054</v>
+        <v>1.6262821429957828</v>
       </c>
       <c r="C2" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A2^2+B2^2, 0)  + _c2*BESSELJ(_c3*A2^2+_c4*B2^2, 0)  - _c5*BESSELJ(_c6*A2^2+_c7*B2^2, 0)</f>
-        <v>2.7732870460328467</v>
+        <f t="shared" ref="C2:C65" ca="1" si="1" xml:space="preserve"> _c1*BESSELJ(A2^2+B2^2, 0)  + _c2*BESSELJ(_c3*A2^2+_c4*B2^2, 0)  - _c5*BESSELJ(_c6*A2^2+_c7*B2^2, 0)</f>
+        <v>-0.44911677577939907</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
@@ -1888,15 +1888,15 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.5762710036582761</v>
+        <v>-0.42224476216435908</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.23419203501158839</v>
+        <v>-0.96627537319928603</v>
       </c>
       <c r="C3" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A3^2+B3^2, 0)  + _c2*BESSELJ(_c3*A3^2+_c4*B3^2, 0)  - _c5*BESSELJ(_c6*A3^2+_c7*B3^2, 0)</f>
-        <v>2.9002796138449107</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.32320825286371002</v>
       </c>
       <c r="F3" t="s">
         <v>1</v>
@@ -1908,15 +1908,15 @@
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.4620440639393224</v>
+        <v>-1.0631895980811197</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52020987089638937</v>
+        <v>-0.15611533479269954</v>
       </c>
       <c r="C4" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A4^2+B4^2, 0)  + _c2*BESSELJ(_c3*A4^2+_c4*B4^2, 0)  - _c5*BESSELJ(_c6*A4^2+_c7*B4^2, 0)</f>
-        <v>-0.12534191177174137</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.11869098887641202</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
@@ -1928,15 +1928,15 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41464517402132572</v>
+        <v>-0.48660711512540394</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5148190333134319E-2</v>
+        <v>-0.61393512132599137</v>
       </c>
       <c r="C5" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A5^2+B5^2, 0)  + _c2*BESSELJ(_c3*A5^2+_c4*B5^2, 0)  - _c5*BESSELJ(_c6*A5^2+_c7*B5^2, 0)</f>
-        <v>3.6665286966834749</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.60890344098413807</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -1948,15 +1948,15 @@
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12021705905178684</v>
+        <v>0.43502732082873846</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1079230189124756</v>
+        <v>-0.55360194292517939</v>
       </c>
       <c r="C6" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A6^2+B6^2, 0)  + _c2*BESSELJ(_c3*A6^2+_c4*B6^2, 0)  - _c5*BESSELJ(_c6*A6^2+_c7*B6^2, 0)</f>
-        <v>2.9855841924598261</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.29166930862400808</v>
       </c>
       <c r="F6" t="s">
         <v>4</v>
@@ -1968,15 +1968,15 @@
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.5937194062495178</v>
+        <v>0.53324420032048947</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.28436742853081737</v>
+        <v>-4.3794451479383462E-2</v>
       </c>
       <c r="C7" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A7^2+B7^2, 0)  + _c2*BESSELJ(_c3*A7^2+_c4*B7^2, 0)  - _c5*BESSELJ(_c6*A7^2+_c7*B7^2, 0)</f>
-        <v>2.1575067200271034</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.1593257593698159</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
@@ -1988,15 +1988,15 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14670458156519092</v>
+        <v>-0.41233474008767595</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.22488668788463281</v>
+        <v>0.1328415643853979</v>
       </c>
       <c r="C8" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A8^2+B8^2, 0)  + _c2*BESSELJ(_c3*A8^2+_c4*B8^2, 0)  - _c5*BESSELJ(_c6*A8^2+_c7*B8^2, 0)</f>
-        <v>2.7227923544946337</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.5560825641778551</v>
       </c>
       <c r="F8" t="s">
         <v>6</v>
@@ -2008,3042 +2008,3042 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.1240500615357783</v>
+        <v>1.9642320536242371E-2</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.1612254929131062E-2</v>
+        <v>8.8732243786034157E-2</v>
       </c>
       <c r="C9" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A9^2+B9^2, 0)  + _c2*BESSELJ(_c3*A9^2+_c4*B9^2, 0)  - _c5*BESSELJ(_c6*A9^2+_c7*B9^2, 0)</f>
-        <v>3.0036452003466843</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.9939186043234285</v>
       </c>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.84692738641670595</v>
+        <v>0.21043058546529897</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14713841720605808</v>
+        <v>0.21196910054639942</v>
       </c>
       <c r="C10" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A10^2+B10^2, 0)  + _c2*BESSELJ(_c3*A10^2+_c4*B10^2, 0)  - _c5*BESSELJ(_c6*A10^2+_c7*B10^2, 0)</f>
-        <v>-0.86835567185362439</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.7784794667970365</v>
       </c>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>7.9953655314593669E-2</v>
+        <v>0.47625948573788013</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.26871162876105342</v>
+        <v>0.86528050184041172</v>
       </c>
       <c r="C11" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A11^2+B11^2, 0)  + _c2*BESSELJ(_c3*A11^2+_c4*B11^2, 0)  - _c5*BESSELJ(_c6*A11^2+_c7*B11^2, 0)</f>
-        <v>2.4978911920644915</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6929556707169962</v>
       </c>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.70470033088692996</v>
+        <v>0.64024759384689711</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.79877848288252173</v>
+        <v>-0.22825827393665263</v>
       </c>
       <c r="C12" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A12^2+B12^2, 0)  + _c2*BESSELJ(_c3*A12^2+_c4*B12^2, 0)  - _c5*BESSELJ(_c6*A12^2+_c7*B12^2, 0)</f>
-        <v>0.42084678159294453</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.2133301763035584</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18089497157356541</v>
+        <v>-0.5352557949653326</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.11116581594692632</v>
+        <v>-0.51406933106994512</v>
       </c>
       <c r="C13" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A13^2+B13^2, 0)  + _c2*BESSELJ(_c3*A13^2+_c4*B13^2, 0)  - _c5*BESSELJ(_c6*A13^2+_c7*B13^2, 0)</f>
-        <v>3.0008085358552377</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.10922675344845945</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.20505962604976261</v>
+        <v>-0.16712368932137781</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.22673404329388674</v>
+        <v>-0.35072817819359131</v>
       </c>
       <c r="C14" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A14^2+B14^2, 0)  + _c2*BESSELJ(_c3*A14^2+_c4*B14^2, 0)  - _c5*BESSELJ(_c6*A14^2+_c7*B14^2, 0)</f>
-        <v>2.7074528579379518</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.5912895423861737</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.33085764942288415</v>
+        <v>0.42957506312280636</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>1.402372360341002E-2</v>
+        <v>-0.63278670196671571</v>
       </c>
       <c r="C15" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A15^2+B15^2, 0)  + _c2*BESSELJ(_c3*A15^2+_c4*B15^2, 0)  - _c5*BESSELJ(_c6*A15^2+_c7*B15^2, 0)</f>
-        <v>3.3621648233025581</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.43782668402587854</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.17650777195480288</v>
+        <v>0.24594079882760636</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3114436561826812</v>
+        <v>-0.76837353798508834</v>
       </c>
       <c r="C16" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A16^2+B16^2, 0)  + _c2*BESSELJ(_c3*A16^2+_c4*B16^2, 0)  - _c5*BESSELJ(_c6*A16^2+_c7*B16^2, 0)</f>
-        <v>-0.11956685119812618</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6220494612115526</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.77769302461114986</v>
+        <v>0.61154951362781584</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6081901669644455</v>
+        <v>-0.22605884836493886</v>
       </c>
       <c r="C17" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A17^2+B17^2, 0)  + _c2*BESSELJ(_c3*A17^2+_c4*B17^2, 0)  - _c5*BESSELJ(_c6*A17^2+_c7*B17^2, 0)</f>
-        <v>0.90963372496127559</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.6387612191986651</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.19533728538586212</v>
+        <v>-0.33658660893896242</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.33128916928171448</v>
+        <v>-0.28534790097256219</v>
       </c>
       <c r="C18" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A18^2+B18^2, 0)  + _c2*BESSELJ(_c3*A18^2+_c4*B18^2, 0)  - _c5*BESSELJ(_c6*A18^2+_c7*B18^2, 0)</f>
-        <v>1.8226210134660816</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.380139760816808</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.71889991115895746</v>
+        <v>-2.0627343365498433E-2</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.11492462086416314</v>
+        <v>0.23687131674591</v>
       </c>
       <c r="C19" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A19^2+B19^2, 0)  + _c2*BESSELJ(_c3*A19^2+_c4*B19^2, 0)  - _c5*BESSELJ(_c6*A19^2+_c7*B19^2, 0)</f>
-        <v>1.5891259748585016</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.7035561720199226</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11012741239590558</v>
+        <v>-0.17885353377201893</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.14596609445937975</v>
+        <v>-0.42868988304505334</v>
       </c>
       <c r="C20" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A20^2+B20^2, 0)  + _c2*BESSELJ(_c3*A20^2+_c4*B20^2, 0)  - _c5*BESSELJ(_c6*A20^2+_c7*B20^2, 0)</f>
-        <v>2.9487046239338142</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.32509199305835734</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.0908618504691583</v>
+        <v>-0.11002436326500646</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2703696876206465</v>
+        <v>-0.72965778516755309</v>
       </c>
       <c r="C21" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A21^2+B21^2, 0)  + _c2*BESSELJ(_c3*A21^2+_c4*B21^2, 0)  - _c5*BESSELJ(_c6*A21^2+_c7*B21^2, 0)</f>
-        <v>0.45187570475374306</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-5.0576468746648895E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22">
-        <f t="shared" ref="A22:B41" ca="1" si="1">_xlfn.NORM.INV(RAND(),0,0.5)</f>
-        <v>0.27029751471900104</v>
+        <f t="shared" ref="A22:B41" ca="1" si="2">_xlfn.NORM.INV(RAND(),0,0.5)</f>
+        <v>0.22186229643367467</v>
       </c>
       <c r="B22">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.86765423639265293</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.37526200918213576</v>
       </c>
       <c r="C22" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A22^2+B22^2, 0)  + _c2*BESSELJ(_c3*A22^2+_c4*B22^2, 0)  - _c5*BESSELJ(_c6*A22^2+_c7*B22^2, 0)</f>
-        <v>2.1942424948907955</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.1979109243103543</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.58724032000358084</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.84291770288542467</v>
       </c>
       <c r="B23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.37245564680953319</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-1.0128442173606973</v>
       </c>
       <c r="C23" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A23^2+B23^2, 0)  + _c2*BESSELJ(_c3*A23^2+_c4*B23^2, 0)  - _c5*BESSELJ(_c6*A23^2+_c7*B23^2, 0)</f>
-        <v>1.0627342604210592</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.7279937526903741</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.46951455374586054</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.28150574719908966</v>
       </c>
       <c r="B24">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.23703266806459669</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.82071534548218539</v>
       </c>
       <c r="C24" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A24^2+B24^2, 0)  + _c2*BESSELJ(_c3*A24^2+_c4*B24^2, 0)  - _c5*BESSELJ(_c6*A24^2+_c7*B24^2, 0)</f>
-        <v>3.119891543716566</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.4437040293764092</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.35728435548544019</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.86904773466097696</v>
       </c>
       <c r="B25">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.43776668791471529</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.17173113616732996</v>
       </c>
       <c r="C25" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A25^2+B25^2, 0)  + _c2*BESSELJ(_c3*A25^2+_c4*B25^2, 0)  - _c5*BESSELJ(_c6*A25^2+_c7*B25^2, 0)</f>
-        <v>0.30871192802972636</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-1.0289251527281449</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9315082782034997E-2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.49036010123430207</v>
       </c>
       <c r="B26">
-        <f t="shared" ca="1" si="1"/>
-        <v>-6.7126037541978142E-2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.38441549486286503</v>
       </c>
       <c r="C26" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A26^2+B26^2, 0)  + _c2*BESSELJ(_c3*A26^2+_c4*B26^2, 0)  - _c5*BESSELJ(_c6*A26^2+_c7*B26^2, 0)</f>
-        <v>2.9979760751857483</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.2995831700129603</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.23083661674829592</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.77877252422577958</v>
       </c>
       <c r="B27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.26258794272866859</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.78002071919733329</v>
       </c>
       <c r="C27" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A27^2+B27^2, 0)  + _c2*BESSELJ(_c3*A27^2+_c4*B27^2, 0)  - _c5*BESSELJ(_c6*A27^2+_c7*B27^2, 0)</f>
-        <v>2.4864004923777467</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.42718655214413542</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.57966177278319941</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.55386211411104291</v>
       </c>
       <c r="B28">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.59378106505525585</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.46112214449124872</v>
       </c>
       <c r="C28" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A28^2+B28^2, 0)  + _c2*BESSELJ(_c3*A28^2+_c4*B28^2, 0)  - _c5*BESSELJ(_c6*A28^2+_c7*B28^2, 0)</f>
-        <v>0.68542046474241125</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.31077077586650104</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29">
-        <f t="shared" ca="1" si="1"/>
-        <v>-5.1344459751715719E-2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.498914275220136E-3</v>
       </c>
       <c r="B29">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.1217392040551961</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>9.2442285780412498E-2</v>
       </c>
       <c r="C29" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A29^2+B29^2, 0)  + _c2*BESSELJ(_c3*A29^2+_c4*B29^2, 0)  - _c5*BESSELJ(_c6*A29^2+_c7*B29^2, 0)</f>
-        <v>2.0920198293957255</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.9930100360112504</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.44212468342560168</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.57043933530171842</v>
       </c>
       <c r="B30">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.7737958832980809E-2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>8.8276162558176816E-2</v>
       </c>
       <c r="C30" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A30^2+B30^2, 0)  + _c2*BESSELJ(_c3*A30^2+_c4*B30^2, 0)  - _c5*BESSELJ(_c6*A30^2+_c7*B30^2, 0)</f>
-        <v>3.8933883195802852</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.9624811908987314</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.57263891919041965</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.22233211057630789</v>
       </c>
       <c r="B31">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.46605218477973515</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.92595253033698255</v>
       </c>
       <c r="C31" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A31^2+B31^2, 0)  + _c2*BESSELJ(_c3*A31^2+_c4*B31^2, 0)  - _c5*BESSELJ(_c6*A31^2+_c7*B31^2, 0)</f>
-        <v>0.21734692298167213</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.2414303869240368</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.91161608165632146</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.73317299262625069</v>
       </c>
       <c r="B32">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.12482174125399459</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.31434023826104762</v>
       </c>
       <c r="C32" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A32^2+B32^2, 0)  + _c2*BESSELJ(_c3*A32^2+_c4*B32^2, 0)  - _c5*BESSELJ(_c6*A32^2+_c7*B32^2, 0)</f>
-        <v>-0.8419272085166809</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.41338192777549354</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.52199485929119593</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.50303395748299384</v>
       </c>
       <c r="B33">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.10149641229413769</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.0838602012197911</v>
       </c>
       <c r="C33" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A33^2+B33^2, 0)  + _c2*BESSELJ(_c3*A33^2+_c4*B33^2, 0)  - _c5*BESSELJ(_c6*A33^2+_c7*B33^2, 0)</f>
-        <v>4.0118267881769851</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.95697649525580675</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34">
-        <f t="shared" ca="1" si="1"/>
-        <v>9.9328481462708881E-2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-7.1296055208927497E-2</v>
       </c>
       <c r="B34">
-        <f t="shared" ca="1" si="1"/>
-        <v>-6.917843009553612E-2</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.23648955411754502</v>
       </c>
       <c r="C34" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A34^2+B34^2, 0)  + _c2*BESSELJ(_c3*A34^2+_c4*B34^2, 0)  - _c5*BESSELJ(_c6*A34^2+_c7*B34^2, 0)</f>
-        <v>2.9987064785871982</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.6939396885756492</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.26147933587209637</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1.3845555102075078</v>
       </c>
       <c r="B35">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.46654058974248153</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.62136603527879275</v>
       </c>
       <c r="C35" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A35^2+B35^2, 0)  + _c2*BESSELJ(_c3*A35^2+_c4*B35^2, 0)  - _c5*BESSELJ(_c6*A35^2+_c7*B35^2, 0)</f>
-        <v>-0.31500621051566313</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.46380875781258374</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.60725108736299716</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.67997882196931692</v>
       </c>
       <c r="B36">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.29583995534796792</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.81164453717708296</v>
       </c>
       <c r="C36" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A36^2+B36^2, 0)  + _c2*BESSELJ(_c3*A36^2+_c4*B36^2, 0)  - _c5*BESSELJ(_c6*A36^2+_c7*B36^2, 0)</f>
-        <v>1.8631888240996828</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.39780755836518567</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.6601020360904416</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.5699747226862153</v>
       </c>
       <c r="B37">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.48187099737202532</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-9.5071659165138794E-2</v>
       </c>
       <c r="C37" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A37^2+B37^2, 0)  + _c2*BESSELJ(_c3*A37^2+_c4*B37^2, 0)  - _c5*BESSELJ(_c6*A37^2+_c7*B37^2, 0)</f>
-        <v>-0.35718506825813795</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.9393454655267774</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.63524286913339045</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.320778024252244</v>
       </c>
       <c r="B38">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.14916598547540932</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.50518195119622933</v>
       </c>
       <c r="C38" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A38^2+B38^2, 0)  + _c2*BESSELJ(_c3*A38^2+_c4*B38^2, 0)  - _c5*BESSELJ(_c6*A38^2+_c7*B38^2, 0)</f>
-        <v>3.0067838610125723</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.70801704273421051</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39">
-        <f t="shared" ca="1" si="1"/>
-        <v>-1.6403284032701597</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.1271029963538215E-2</v>
       </c>
       <c r="B39">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.22203918173041456</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.41315644753334696</v>
       </c>
       <c r="C39" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A39^2+B39^2, 0)  + _c2*BESSELJ(_c3*A39^2+_c4*B39^2, 0)  - _c5*BESSELJ(_c6*A39^2+_c7*B39^2, 0)</f>
-        <v>-0.77605194223857343</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.69017603618563172</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.45722752242791442</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0.25485512205909461</v>
       </c>
       <c r="B40">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.25381005366892306</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.58429175074554096</v>
       </c>
       <c r="C40" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A40^2+B40^2, 0)  + _c2*BESSELJ(_c3*A40^2+_c4*B40^2, 0)  - _c5*BESSELJ(_c6*A40^2+_c7*B40^2, 0)</f>
-        <v>2.9436943811443603</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-1.4578741605122807</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.50488085178690822</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.15563726006397283</v>
       </c>
       <c r="B41">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.14341722817482011</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>-0.31141736770919698</v>
       </c>
       <c r="C41" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A41^2+B41^2, 0)  + _c2*BESSELJ(_c3*A41^2+_c4*B41^2, 0)  - _c5*BESSELJ(_c6*A41^2+_c7*B41^2, 0)</f>
-        <v>3.8185937875084117</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.0765194067158306</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42">
-        <f t="shared" ref="A42:B61" ca="1" si="2">_xlfn.NORM.INV(RAND(),0,0.5)</f>
-        <v>0.34556753004297669</v>
+        <f t="shared" ref="A42:B61" ca="1" si="3">_xlfn.NORM.INV(RAND(),0,0.5)</f>
+        <v>-5.7818969598847129E-2</v>
       </c>
       <c r="B42">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.31028695011486168</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-1.0326216401431791</v>
       </c>
       <c r="C42" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A42^2+B42^2, 0)  + _c2*BESSELJ(_c3*A42^2+_c4*B42^2, 0)  - _c5*BESSELJ(_c6*A42^2+_c7*B42^2, 0)</f>
-        <v>2.1249899571971747</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.5135686688458958</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.94396064033456462</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.23530520526209037</v>
       </c>
       <c r="B43">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.3331860258956455</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-7.2584424258814922E-2</v>
       </c>
       <c r="C43" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A43^2+B43^2, 0)  + _c2*BESSELJ(_c3*A43^2+_c4*B43^2, 0)  - _c5*BESSELJ(_c6*A43^2+_c7*B43^2, 0)</f>
-        <v>-4.9196632032103671E-2</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.083172551198325</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.52983755580631342</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.23698347209297965</v>
       </c>
       <c r="B44">
-        <f t="shared" ca="1" si="2"/>
-        <v>-1.0140806339228573E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.63419776734228994</v>
       </c>
       <c r="C44" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A44^2+B44^2, 0)  + _c2*BESSELJ(_c3*A44^2+_c4*B44^2, 0)  - _c5*BESSELJ(_c6*A44^2+_c7*B44^2, 0)</f>
-        <v>4.1897143245995574</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-1.2475753483084397</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.2988070342330838</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-1.4029287028622717</v>
       </c>
       <c r="B45">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.22778834148788826</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.32542344989274402</v>
       </c>
       <c r="C45" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A45^2+B45^2, 0)  + _c2*BESSELJ(_c3*A45^2+_c4*B45^2, 0)  - _c5*BESSELJ(_c6*A45^2+_c7*B45^2, 0)</f>
-        <v>2.7767075081885344</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.4461320569505931</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.14018891200631001</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.23519106595801467</v>
       </c>
       <c r="B46">
-        <f t="shared" ca="1" si="2"/>
-        <v>-2.4313537155593753E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.96420271629001841</v>
       </c>
       <c r="C46" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A46^2+B46^2, 0)  + _c2*BESSELJ(_c3*A46^2+_c4*B46^2, 0)  - _c5*BESSELJ(_c6*A46^2+_c7*B46^2, 0)</f>
-        <v>3.0123702929511795</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.69097757060174003</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.31254863224951851</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.74919365991532838</v>
       </c>
       <c r="B47">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.3625024119825879E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.53415015562114143</v>
       </c>
       <c r="C47" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A47^2+B47^2, 0)  + _c2*BESSELJ(_c3*A47^2+_c4*B47^2, 0)  - _c5*BESSELJ(_c6*A47^2+_c7*B47^2, 0)</f>
-        <v>3.2803229250273795</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.26124374972085607</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.15797212090571633</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.44658871670553535</v>
       </c>
       <c r="B48">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.54010846429065873</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.74600694983731108</v>
       </c>
       <c r="C48" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A48^2+B48^2, 0)  + _c2*BESSELJ(_c3*A48^2+_c4*B48^2, 0)  - _c5*BESSELJ(_c6*A48^2+_c7*B48^2, 0)</f>
-        <v>-1.5037531465895331</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.6018408058318183</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.33546654343055815</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>9.1142512195508674E-2</v>
       </c>
       <c r="B49">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.49929708673703976</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.37901476093219333</v>
       </c>
       <c r="C49" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A49^2+B49^2, 0)  + _c2*BESSELJ(_c3*A49^2+_c4*B49^2, 0)  - _c5*BESSELJ(_c6*A49^2+_c7*B49^2, 0)</f>
-        <v>-0.58786733073589159</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.2387393498980082</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50">
-        <f t="shared" ca="1" si="2"/>
-        <v>8.7029913037801235E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.25036271051446291</v>
       </c>
       <c r="B50">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.39764335199805217</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.44700068566820594</v>
       </c>
       <c r="C50" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A50^2+B50^2, 0)  + _c2*BESSELJ(_c3*A50^2+_c4*B50^2, 0)  - _c5*BESSELJ(_c6*A50^2+_c7*B50^2, 0)</f>
-        <v>0.93698638017831803</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.9474752490752394E-4</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A51">
-        <f t="shared" ca="1" si="2"/>
-        <v>9.1316659058379199E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-1.9845682222020461E-2</v>
       </c>
       <c r="B51">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.21409637253534317</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.60872247894297316</v>
       </c>
       <c r="C51" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A51^2+B51^2, 0)  + _c2*BESSELJ(_c3*A51^2+_c4*B51^2, 0)  - _c5*BESSELJ(_c6*A51^2+_c7*B51^2, 0)</f>
-        <v>2.7854239693919345</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-2.0570047997014171</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A52">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.72011854797374752</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.28639315414110017</v>
       </c>
       <c r="B52">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.28444580360448735</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.70034552095020008</v>
       </c>
       <c r="C52" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A52^2+B52^2, 0)  + _c2*BESSELJ(_c3*A52^2+_c4*B52^2, 0)  - _c5*BESSELJ(_c6*A52^2+_c7*B52^2, 0)</f>
-        <v>0.10286640144545596</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.40375335537451656</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.32290890269035483</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-1.0651414143115843</v>
       </c>
       <c r="B53">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.86445041491701102</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2.0433939085933925E-2</v>
       </c>
       <c r="C53" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A53^2+B53^2, 0)  + _c2*BESSELJ(_c3*A53^2+_c4*B53^2, 0)  - _c5*BESSELJ(_c6*A53^2+_c7*B53^2, 0)</f>
-        <v>2.2947673859228015</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.33514230881296214</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54">
-        <f t="shared" ca="1" si="2"/>
-        <v>6.2652431546649456E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-5.7083179630207275E-3</v>
       </c>
       <c r="B54">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.11862382582573137</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.59428705355710809</v>
       </c>
       <c r="C54" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A54^2+B54^2, 0)  + _c2*BESSELJ(_c3*A54^2+_c4*B54^2, 0)  - _c5*BESSELJ(_c6*A54^2+_c7*B54^2, 0)</f>
-        <v>2.9788071618353804</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-2.0447078600543085</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55">
-        <f t="shared" ca="1" si="2"/>
-        <v>1.3219533774636172</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-2.380769051654559E-2</v>
       </c>
       <c r="B55">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.88900418851449081</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-2.9083596435117882E-2</v>
       </c>
       <c r="C55" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A55^2+B55^2, 0)  + _c2*BESSELJ(_c3*A55^2+_c4*B55^2, 0)  - _c5*BESSELJ(_c6*A55^2+_c7*B55^2, 0)</f>
-        <v>-0.38673506981616879</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.9999181340743011</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A56">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.39024574894699932</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.62336611330374503</v>
       </c>
       <c r="B56">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.8717593390412538</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.40398429603354108</v>
       </c>
       <c r="C56" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A56^2+B56^2, 0)  + _c2*BESSELJ(_c3*A56^2+_c4*B56^2, 0)  - _c5*BESSELJ(_c6*A56^2+_c7*B56^2, 0)</f>
-        <v>2.0874583634099881</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.35324380636242525</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A57">
-        <f t="shared" ca="1" si="2"/>
-        <v>-6.8439215599265954E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.39386506408097083</v>
       </c>
       <c r="B57">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.57809998097686066</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.64047323911417608</v>
       </c>
       <c r="C57" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A57^2+B57^2, 0)  + _c2*BESSELJ(_c3*A57^2+_c4*B57^2, 0)  - _c5*BESSELJ(_c6*A57^2+_c7*B57^2, 0)</f>
-        <v>-1.9423549707975318</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.22491901035135581</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A58">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.7416140353990216</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.26781539163498846</v>
       </c>
       <c r="B58">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.26273202899731746</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.98001116190861104</v>
       </c>
       <c r="C58" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A58^2+B58^2, 0)  + _c2*BESSELJ(_c3*A58^2+_c4*B58^2, 0)  - _c5*BESSELJ(_c6*A58^2+_c7*B58^2, 0)</f>
-        <v>-0.10042984619475513</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.57524229015079131</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A59">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.37642620307468572</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.44349617280124104</v>
       </c>
       <c r="B59">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.52074039450957554</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.57736575145877267</v>
       </c>
       <c r="C59" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A59^2+B59^2, 0)  + _c2*BESSELJ(_c3*A59^2+_c4*B59^2, 0)  - _c5*BESSELJ(_c6*A59^2+_c7*B59^2, 0)</f>
-        <v>-0.58695475459696844</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.11773941220735962</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A60">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.32446144289201706</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0.53775108821683371</v>
       </c>
       <c r="B60">
-        <f t="shared" ca="1" si="2"/>
-        <v>-2.3124036303876203E-2</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-1.0220774066536786</v>
       </c>
       <c r="C60" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A60^2+B60^2, 0)  + _c2*BESSELJ(_c3*A60^2+_c4*B60^2, 0)  - _c5*BESSELJ(_c6*A60^2+_c7*B60^2, 0)</f>
-        <v>3.335788551770773</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>0.11137446749702734</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A61">
-        <f t="shared" ca="1" si="2"/>
-        <v>0.25849698795607012</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.13945231196476182</v>
       </c>
       <c r="B61">
-        <f t="shared" ca="1" si="2"/>
-        <v>-0.47388994603139228</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>-0.17454757367432272</v>
       </c>
       <c r="C61" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A61^2+B61^2, 0)  + _c2*BESSELJ(_c3*A61^2+_c4*B61^2, 0)  - _c5*BESSELJ(_c6*A61^2+_c7*B61^2, 0)</f>
-        <v>-0.43644296643897273</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.8950888238751915</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A62">
-        <f t="shared" ref="A62:B81" ca="1" si="3">_xlfn.NORM.INV(RAND(),0,0.5)</f>
-        <v>0.34334623009949605</v>
+        <f t="shared" ref="A62:B81" ca="1" si="4">_xlfn.NORM.INV(RAND(),0,0.5)</f>
+        <v>0.39357602709812001</v>
       </c>
       <c r="B62">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.60986359554162939</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.38501295111895678</v>
       </c>
       <c r="C62" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A62^2+B62^2, 0)  + _c2*BESSELJ(_c3*A62^2+_c4*B62^2, 0)  - _c5*BESSELJ(_c6*A62^2+_c7*B62^2, 0)</f>
-        <v>-0.68715766643423504</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.1841152357479872</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A63">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.77055652088984938</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.46021058062886783</v>
       </c>
       <c r="B63">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.40839200676460485</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-5.221206142830534E-2</v>
       </c>
       <c r="C63" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A63^2+B63^2, 0)  + _c2*BESSELJ(_c3*A63^2+_c4*B63^2, 0)  - _c5*BESSELJ(_c6*A63^2+_c7*B63^2, 0)</f>
-        <v>-1.2153502974666077</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.9560608075179444</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A64">
-        <f t="shared" ca="1" si="3"/>
-        <v>3.0726839440882456E-3</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>5.4637151291457688E-3</v>
       </c>
       <c r="B64">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.33210640062549118</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.1412152129226916</v>
       </c>
       <c r="C64" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A64^2+B64^2, 0)  + _c2*BESSELJ(_c3*A64^2+_c4*B64^2, 0)  - _c5*BESSELJ(_c6*A64^2+_c7*B64^2, 0)</f>
-        <v>1.9242215087051724</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.9619913599300607</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A65">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.65269130404981057</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.41239439064884209</v>
       </c>
       <c r="B65">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.71563649830403764</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.33613520699519994</v>
       </c>
       <c r="C65" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A65^2+B65^2, 0)  + _c2*BESSELJ(_c3*A65^2+_c4*B65^2, 0)  - _c5*BESSELJ(_c6*A65^2+_c7*B65^2, 0)</f>
-        <v>1.7891918866222689</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>1.9142590004360089</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.44649881808350672</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.55084247980990508</v>
       </c>
       <c r="B66">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.41171115791886642</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.74179834865295025</v>
       </c>
       <c r="C66" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A66^2+B66^2, 0)  + _c2*BESSELJ(_c3*A66^2+_c4*B66^2, 0)  - _c5*BESSELJ(_c6*A66^2+_c7*B66^2, 0)</f>
-        <v>0.8865509978896835</v>
+        <f t="shared" ref="C66:C129" ca="1" si="5" xml:space="preserve"> _c1*BESSELJ(A66^2+B66^2, 0)  + _c2*BESSELJ(_c3*A66^2+_c4*B66^2, 0)  - _c5*BESSELJ(_c6*A66^2+_c7*B66^2, 0)</f>
+        <v>2.5192206939133142</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67">
-        <f t="shared" ca="1" si="3"/>
-        <v>-5.2972436701440209E-2</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.15066129885042581</v>
       </c>
       <c r="B67">
-        <f t="shared" ca="1" si="3"/>
-        <v>-6.2477818049949181E-2</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.31299405568230027</v>
       </c>
       <c r="C67" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A67^2+B67^2, 0)  + _c2*BESSELJ(_c3*A67^2+_c4*B67^2, 0)  - _c5*BESSELJ(_c6*A67^2+_c7*B67^2, 0)</f>
-        <v>2.9982539730944104</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.0633774664229594</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A68">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.15065807542035412</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.39224166305194741</v>
       </c>
       <c r="B68">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.50458258881356477</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>8.4759918705619615E-4</v>
       </c>
       <c r="C68" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A68^2+B68^2, 0)  + _c2*BESSELJ(_c3*A68^2+_c4*B68^2, 0)  - _c5*BESSELJ(_c6*A68^2+_c7*B68^2, 0)</f>
-        <v>-1.0134180630129497</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>3.6437667606058115</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A69">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.38612182270511952</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.56592623846438517</v>
       </c>
       <c r="B69">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.25229603259772609</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.27206151533715878</v>
       </c>
       <c r="C69" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A69^2+B69^2, 0)  + _c2*BESSELJ(_c3*A69^2+_c4*B69^2, 0)  - _c5*BESSELJ(_c6*A69^2+_c7*B69^2, 0)</f>
-        <v>2.7902312960751825</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.5452948412063745</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A70">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.29096382667144954</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.21702091467405749</v>
       </c>
       <c r="B70">
-        <f t="shared" ca="1" si="3"/>
-        <v>-9.9941994451747784E-2</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-1.0843556101070648</v>
       </c>
       <c r="C70" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A70^2+B70^2, 0)  + _c2*BESSELJ(_c3*A70^2+_c4*B70^2, 0)  - _c5*BESSELJ(_c6*A70^2+_c7*B70^2, 0)</f>
-        <v>3.173879880401393</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.5968748793067435</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A71">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.49432698578141215</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.2203307996659046</v>
       </c>
       <c r="B71">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.88967826811099016</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>1.7809174684136928E-2</v>
       </c>
       <c r="C71" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A71^2+B71^2, 0)  + _c2*BESSELJ(_c3*A71^2+_c4*B71^2, 0)  - _c5*BESSELJ(_c6*A71^2+_c7*B71^2, 0)</f>
-        <v>0.96559966067564629</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>3.0771078166706469</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A72">
-        <f t="shared" ca="1" si="3"/>
-        <v>-1.1058883788903069</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.42109726474246539</v>
       </c>
       <c r="B72">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.23449719338019687</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.56778436435029367</v>
       </c>
       <c r="C72" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A72^2+B72^2, 0)  + _c2*BESSELJ(_c3*A72^2+_c4*B72^2, 0)  - _c5*BESSELJ(_c6*A72^2+_c7*B72^2, 0)</f>
-        <v>0.26713728943684123</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>-0.34424975716161327</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A73">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.90823794723090623</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.35699929476280651</v>
       </c>
       <c r="B73">
-        <f t="shared" ca="1" si="3"/>
-        <v>-4.4040047482919509E-2</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.15225207513485806</v>
       </c>
       <c r="C73" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A73^2+B73^2, 0)  + _c2*BESSELJ(_c3*A73^2+_c4*B73^2, 0)  - _c5*BESSELJ(_c6*A73^2+_c7*B73^2, 0)</f>
-        <v>-0.77329617476206591</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>3.2691888091224546</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A74">
-        <f t="shared" ca="1" si="3"/>
-        <v>4.558329935318102E-2</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.29951589807598167</v>
       </c>
       <c r="B74">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.65590834780250107</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.17460241808700863</v>
       </c>
       <c r="C74" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A74^2+B74^2, 0)  + _c2*BESSELJ(_c3*A74^2+_c4*B74^2, 0)  - _c5*BESSELJ(_c6*A74^2+_c7*B74^2, 0)</f>
-        <v>-1.7111672728756187</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>3.0274501867917798</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A75">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.12778887208999457</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.22853324928496885</v>
       </c>
       <c r="B75">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.16341178491304884</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.25604921633911099</v>
       </c>
       <c r="C75" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A75^2+B75^2, 0)  + _c2*BESSELJ(_c3*A75^2+_c4*B75^2, 0)  - _c5*BESSELJ(_c6*A75^2+_c7*B75^2, 0)</f>
-        <v>2.9193528271667302</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.533552530533659</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A76">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.12447933342870864</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.26955398867956887</v>
       </c>
       <c r="B76">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.67094295334815612</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-1.0678824057001501</v>
       </c>
       <c r="C76" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A76^2+B76^2, 0)  + _c2*BESSELJ(_c3*A76^2+_c4*B76^2, 0)  - _c5*BESSELJ(_c6*A76^2+_c7*B76^2, 0)</f>
-        <v>-1.292289691797996</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.3406984456320181</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A77">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.77590028000344413</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-5.9072657656355769E-2</v>
       </c>
       <c r="B77">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.17689961548094676</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.2375658210863883</v>
       </c>
       <c r="C77" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A77^2+B77^2, 0)  + _c2*BESSELJ(_c3*A77^2+_c4*B77^2, 0)  - _c5*BESSELJ(_c6*A77^2+_c7*B77^2, 0)</f>
-        <v>-6.6191722696964661E-2</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.6923562298121828</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A78">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.12016978222484957</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.86835631594766827</v>
       </c>
       <c r="B78">
-        <f t="shared" ca="1" si="3"/>
-        <v>-0.1785540864529491</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.203738215526199</v>
       </c>
       <c r="C78" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A78^2+B78^2, 0)  + _c2*BESSELJ(_c3*A78^2+_c4*B78^2, 0)  - _c5*BESSELJ(_c6*A78^2+_c7*B78^2, 0)</f>
-        <v>2.887613051667401</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>-1.1124196055844768</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A79">
-        <f t="shared" ca="1" si="3"/>
-        <v>4.8069072224934159E-2</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.7581973574963865</v>
       </c>
       <c r="B79">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.4048502697987113</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.58904166956031923</v>
       </c>
       <c r="C79" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A79^2+B79^2, 0)  + _c2*BESSELJ(_c3*A79^2+_c4*B79^2, 0)  - _c5*BESSELJ(_c6*A79^2+_c7*B79^2, 0)</f>
-        <v>0.83456331468755196</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.5419451459264738</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A80">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.58643641765133936</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.22681236871491528</v>
       </c>
       <c r="B80">
-        <f t="shared" ca="1" si="3"/>
-        <v>7.1693146874904273E-2</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-0.86755871983065513</v>
       </c>
       <c r="C80" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A80^2+B80^2, 0)  + _c2*BESSELJ(_c3*A80^2+_c4*B80^2, 0)  - _c5*BESSELJ(_c6*A80^2+_c7*B80^2, 0)</f>
-        <v>3.9252258643124587</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.106319980638669</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A81">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.30795709290903045</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>0.34934797200064632</v>
       </c>
       <c r="B81">
-        <f t="shared" ca="1" si="3"/>
-        <v>0.32756973069766665</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>-8.2988105315923891E-2</v>
       </c>
       <c r="C81" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A81^2+B81^2, 0)  + _c2*BESSELJ(_c3*A81^2+_c4*B81^2, 0)  - _c5*BESSELJ(_c6*A81^2+_c7*B81^2, 0)</f>
-        <v>1.8717539169303665</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>3.3906330243247638</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82">
-        <f t="shared" ref="A82:B101" ca="1" si="4">_xlfn.NORM.INV(RAND(),0,0.5)</f>
-        <v>0.33269804768283529</v>
+        <f t="shared" ref="A82:B101" ca="1" si="6">_xlfn.NORM.INV(RAND(),0,0.5)</f>
+        <v>5.3433660429425961E-3</v>
       </c>
       <c r="B82">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.83646841878010891</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-5.4305744942288996E-3</v>
       </c>
       <c r="C82" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A82^2+B82^2, 0)  + _c2*BESSELJ(_c3*A82^2+_c4*B82^2, 0)  - _c5*BESSELJ(_c6*A82^2+_c7*B82^2, 0)</f>
-        <v>2.5821232578431568</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.9999999102086425</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.45146750655911566</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.46624663296856805</v>
       </c>
       <c r="B83">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.69621817378131723</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.2917518713349766</v>
       </c>
       <c r="C83" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A83^2+B83^2, 0)  + _c2*BESSELJ(_c3*A83^2+_c4*B83^2, 0)  - _c5*BESSELJ(_c6*A83^2+_c7*B83^2, 0)</f>
-        <v>1.8338085778217339</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.5464198237341829</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.56381299779794047</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.2856546728042597E-2</v>
       </c>
       <c r="B84">
-        <f t="shared" ca="1" si="4"/>
-        <v>-8.3897138751811026E-2</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.25866819575380862</v>
       </c>
       <c r="C84" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A84^2+B84^2, 0)  + _c2*BESSELJ(_c3*A84^2+_c4*B84^2, 0)  - _c5*BESSELJ(_c6*A84^2+_c7*B84^2, 0)</f>
-        <v>4.006184485037398</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.5820561278759433</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85">
-        <f t="shared" ca="1" si="4"/>
-        <v>-6.3559389266872851E-2</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.73433208813671746</v>
       </c>
       <c r="B85">
-        <f t="shared" ca="1" si="4"/>
-        <v>1.0383433973610483</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-6.4447386765648415E-2</v>
       </c>
       <c r="C85" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A85^2+B85^2, 0)  + _c2*BESSELJ(_c3*A85^2+_c4*B85^2, 0)  - _c5*BESSELJ(_c6*A85^2+_c7*B85^2, 0)</f>
-        <v>0.59110414378285125</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.4513351013303755</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A86">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.27244571142535323</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.1282948917071866E-2</v>
       </c>
       <c r="B86">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.71950444535872682</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>7.7661732299986644E-2</v>
       </c>
       <c r="C86" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A86^2+B86^2, 0)  + _c2*BESSELJ(_c3*A86^2+_c4*B86^2, 0)  - _c5*BESSELJ(_c6*A86^2+_c7*B86^2, 0)</f>
-        <v>0.73491252787109385</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.9963867816031753</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.72782863732186265</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.4427214581458091</v>
       </c>
       <c r="B87">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.38479969354196386</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.2880848857466058</v>
       </c>
       <c r="C87" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A87^2+B87^2, 0)  + _c2*BESSELJ(_c3*A87^2+_c4*B87^2, 0)  - _c5*BESSELJ(_c6*A87^2+_c7*B87^2, 0)</f>
-        <v>-0.82511257279191308</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>-0.7811263701548915</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88">
-        <f t="shared" ca="1" si="4"/>
-        <v>8.6636202924687516E-2</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.26024389411912929</v>
       </c>
       <c r="B88">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.58754532023555872</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.15046423220072191</v>
       </c>
       <c r="C88" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A88^2+B88^2, 0)  + _c2*BESSELJ(_c3*A88^2+_c4*B88^2, 0)  - _c5*BESSELJ(_c6*A88^2+_c7*B88^2, 0)</f>
-        <v>-1.9704236552549408</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>3.0226094142154962</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.36167908544042193</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.30523566207597647</v>
       </c>
       <c r="B89">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.79304830733437959</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.19334389736011506</v>
       </c>
       <c r="C89" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A89^2+B89^2, 0)  + _c2*BESSELJ(_c3*A89^2+_c4*B89^2, 0)  - _c5*BESSELJ(_c6*A89^2+_c7*B89^2, 0)</f>
-        <v>2.6740695038794025</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.9663991826089493</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A90">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.48734268225282223</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.17077290770263837</v>
       </c>
       <c r="B90">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.31445429083105558</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.27883960319563661</v>
       </c>
       <c r="C90" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A90^2+B90^2, 0)  + _c2*BESSELJ(_c3*A90^2+_c4*B90^2, 0)  - _c5*BESSELJ(_c6*A90^2+_c7*B90^2, 0)</f>
-        <v>2.2686532445983731</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.3720839479794682</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A91">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.57874759921869168</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.8841793437097798</v>
       </c>
       <c r="B91">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.70651252130463083</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.68855294290886793</v>
       </c>
       <c r="C91" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A91^2+B91^2, 0)  + _c2*BESSELJ(_c3*A91^2+_c4*B91^2, 0)  - _c5*BESSELJ(_c6*A91^2+_c7*B91^2, 0)</f>
-        <v>2.2067829472598186</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.7385815756838996</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A92">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.11000245137421738</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-7.2404234736960296E-2</v>
       </c>
       <c r="B92">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.81893175599925128</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.45883057008887307</v>
       </c>
       <c r="C92" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A92^2+B92^2, 0)  + _c2*BESSELJ(_c3*A92^2+_c4*B92^2, 0)  - _c5*BESSELJ(_c6*A92^2+_c7*B92^2, 0)</f>
-        <v>1.7503223635236105</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>-0.17746586375598872</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A93">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.4908735089668273</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-7.9280035684009278E-2</v>
       </c>
       <c r="B93">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.33272351090869257</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.10391615781596161</v>
       </c>
       <c r="C93" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A93^2+B93^2, 0)  + _c2*BESSELJ(_c3*A93^2+_c4*B93^2, 0)  - _c5*BESSELJ(_c6*A93^2+_c7*B93^2, 0)</f>
-        <v>2.0232971407868963</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.9867574835321471</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.47772917941350751</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.65953948502976256</v>
       </c>
       <c r="B94">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.74982782463195474</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.15339355406995384</v>
       </c>
       <c r="C94" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A94^2+B94^2, 0)  + _c2*BESSELJ(_c3*A94^2+_c4*B94^2, 0)  - _c5*BESSELJ(_c6*A94^2+_c7*B94^2, 0)</f>
-        <v>2.7092165788960401</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.5768958426278337</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A95">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.62910941706217693</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-7.2743462977417031E-2</v>
       </c>
       <c r="B95">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.28188843796860852</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.15640310058813633</v>
       </c>
       <c r="C95" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A95^2+B95^2, 0)  + _c2*BESSELJ(_c3*A95^2+_c4*B95^2, 0)  - _c5*BESSELJ(_c6*A95^2+_c7*B95^2, 0)</f>
-        <v>1.7550881441176367</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.937416056660509</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A96">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.72174502352600034</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.38209161065512265</v>
       </c>
       <c r="B96">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.12539068762728889</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.95339619478693471</v>
       </c>
       <c r="C96" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A96^2+B96^2, 0)  + _c2*BESSELJ(_c3*A96^2+_c4*B96^2, 0)  - _c5*BESSELJ(_c6*A96^2+_c7*B96^2, 0)</f>
-        <v>1.4620901433549045</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.62268738060900497</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A97">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.27558352505055439</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.93649865229000351</v>
       </c>
       <c r="B97">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.13965777775244059</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-1.032035638015758</v>
       </c>
       <c r="C97" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A97^2+B97^2, 0)  + _c2*BESSELJ(_c3*A97^2+_c4*B97^2, 0)  - _c5*BESSELJ(_c6*A97^2+_c7*B97^2, 0)</f>
-        <v>3.0735468857191695</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.76907873627950829</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A98">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.25207094268981262</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.11983061303755858</v>
       </c>
       <c r="B98">
-        <f t="shared" ca="1" si="4"/>
-        <v>4.6260214630029328E-2</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.18839572303536786</v>
       </c>
       <c r="C98" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A98^2+B98^2, 0)  + _c2*BESSELJ(_c3*A98^2+_c4*B98^2, 0)  - _c5*BESSELJ(_c6*A98^2+_c7*B98^2, 0)</f>
-        <v>3.1240711463444808</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.8622771311069899</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A99">
-        <f t="shared" ca="1" si="4"/>
-        <v>0.28840460374719562</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.17065221790549012</v>
       </c>
       <c r="B99">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.16534144147199809</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.92193619293541595</v>
       </c>
       <c r="C99" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A99^2+B99^2, 0)  + _c2*BESSELJ(_c3*A99^2+_c4*B99^2, 0)  - _c5*BESSELJ(_c6*A99^2+_c7*B99^2, 0)</f>
-        <v>3.0341682542711608</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.2600151821078063</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A100">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.4370534133717035</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.30490874749730557</v>
       </c>
       <c r="B100">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.45675842963946051</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>-0.68527635060712921</v>
       </c>
       <c r="C100" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A100^2+B100^2, 0)  + _c2*BESSELJ(_c3*A100^2+_c4*B100^2, 0)  - _c5*BESSELJ(_c6*A100^2+_c7*B100^2, 0)</f>
-        <v>0.27178943873244343</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.23221760558999774</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A101">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.32261475664995082</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.2238525599662353</v>
       </c>
       <c r="B101">
-        <f t="shared" ca="1" si="4"/>
-        <v>-0.28954328774337268</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>3.2845628509963483E-2</v>
       </c>
       <c r="C101" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A101^2+B101^2, 0)  + _c2*BESSELJ(_c3*A101^2+_c4*B101^2, 0)  - _c5*BESSELJ(_c6*A101^2+_c7*B101^2, 0)</f>
-        <v>2.3170691950998892</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.1380961412033319</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102">
-        <f t="shared" ref="A102:B121" ca="1" si="5">_xlfn.NORM.INV(RAND(),0,0.5)</f>
-        <v>0.19802851352033679</v>
+        <f t="shared" ref="A102:B121" ca="1" si="7">_xlfn.NORM.INV(RAND(),0,0.5)</f>
+        <v>0.9182311703510333</v>
       </c>
       <c r="B102">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.16548189489558149</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.66502209164937942</v>
       </c>
       <c r="C102" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A102^2+B102^2, 0)  + _c2*BESSELJ(_c3*A102^2+_c4*B102^2, 0)  - _c5*BESSELJ(_c6*A102^2+_c7*B102^2, 0)</f>
-        <v>2.9264366873788412</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.9496007963503819</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103">
-        <f t="shared" ca="1" si="5"/>
-        <v>-2.2220772878979965E-2</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.92990429097048566</v>
       </c>
       <c r="B103">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.79604887400116486</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.4203053714052758</v>
       </c>
       <c r="C103" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A103^2+B103^2, 0)  + _c2*BESSELJ(_c3*A103^2+_c4*B103^2, 0)  - _c5*BESSELJ(_c6*A103^2+_c7*B103^2, 0)</f>
-        <v>1.2721621694413576</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.60404780106515621</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A104">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.10315912697492344</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.63149185966740695</v>
       </c>
       <c r="B104">
-        <f t="shared" ca="1" si="5"/>
-        <v>1.1712616216786473</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.46207472105816533</v>
       </c>
       <c r="C104" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A104^2+B104^2, 0)  + _c2*BESSELJ(_c3*A104^2+_c4*B104^2, 0)  - _c5*BESSELJ(_c6*A104^2+_c7*B104^2, 0)</f>
-        <v>2.1152472273435361</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>-0.11669938826716775</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A105">
-        <f t="shared" ca="1" si="5"/>
-        <v>-0.2745309842765114</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.62415918321178465</v>
       </c>
       <c r="B105">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.21611440962415068</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-9.6236319474408152E-2</v>
       </c>
       <c r="C105" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A105^2+B105^2, 0)  + _c2*BESSELJ(_c3*A105^2+_c4*B105^2, 0)  - _c5*BESSELJ(_c6*A105^2+_c7*B105^2, 0)</f>
-        <v>2.807021380775216</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>3.4678476803389255</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A106">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.32587709474611659</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.55663102499870898</v>
       </c>
       <c r="B106">
-        <f t="shared" ca="1" si="5"/>
-        <v>-0.36732446950329667</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.66339821550671718</v>
       </c>
       <c r="C106" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A106^2+B106^2, 0)  + _c2*BESSELJ(_c3*A106^2+_c4*B106^2, 0)  - _c5*BESSELJ(_c6*A106^2+_c7*B106^2, 0)</f>
-        <v>1.3451738581476431</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.7026183138927073</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107">
-        <f t="shared" ca="1" si="5"/>
-        <v>-0.16645284268241597</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.73036391416055224</v>
       </c>
       <c r="B107">
-        <f t="shared" ca="1" si="5"/>
-        <v>-5.2964363903808466E-2</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.12972649497959826</v>
       </c>
       <c r="C107" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A107^2+B107^2, 0)  + _c2*BESSELJ(_c3*A107^2+_c4*B107^2, 0)  - _c5*BESSELJ(_c6*A107^2+_c7*B107^2, 0)</f>
-        <v>3.0210459468366908</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.236454801444024</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A108">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.52169452677383099</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.87270851847585151</v>
       </c>
       <c r="B108">
-        <f t="shared" ca="1" si="5"/>
-        <v>-0.37887654488357947</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>8.4992071968483268E-2</v>
       </c>
       <c r="C108" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A108^2+B108^2, 0)  + _c2*BESSELJ(_c3*A108^2+_c4*B108^2, 0)  - _c5*BESSELJ(_c6*A108^2+_c7*B108^2, 0)</f>
-        <v>1.3305571174796418</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>-0.82373954993519738</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A109">
-        <f t="shared" ca="1" si="5"/>
-        <v>-0.14999499617305559</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.12517103802544741</v>
       </c>
       <c r="B109">
-        <f t="shared" ca="1" si="5"/>
-        <v>1.731823630120979E-2</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.94010613833073031</v>
       </c>
       <c r="C109" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A109^2+B109^2, 0)  + _c2*BESSELJ(_c3*A109^2+_c4*B109^2, 0)  - _c5*BESSELJ(_c6*A109^2+_c7*B109^2, 0)</f>
-        <v>3.0166577259808953</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.92271314821739381</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A110">
-        <f t="shared" ca="1" si="5"/>
-        <v>-7.8034653631727083E-2</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.62068232237043663</v>
       </c>
       <c r="B110">
-        <f t="shared" ca="1" si="5"/>
-        <v>-1.0544288788280876</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>8.6805563152833748E-3</v>
       </c>
       <c r="C110" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A110^2+B110^2, 0)  + _c2*BESSELJ(_c3*A110^2+_c4*B110^2, 0)  - _c5*BESSELJ(_c6*A110^2+_c7*B110^2, 0)</f>
-        <v>0.86040021334185002</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>3.722257021308871</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A111">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.81495671944217873</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.20944130863072857</v>
       </c>
       <c r="B111">
-        <f t="shared" ca="1" si="5"/>
-        <v>6.9947820544135286E-2</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.37154050180640935</v>
       </c>
       <c r="C111" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A111^2+B111^2, 0)  + _c2*BESSELJ(_c3*A111^2+_c4*B111^2, 0)  - _c5*BESSELJ(_c6*A111^2+_c7*B111^2, 0)</f>
-        <v>-0.24959661563267521</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.2609275807199698</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A112">
-        <f t="shared" ca="1" si="5"/>
-        <v>-0.47924632513479232</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.75385052912937356</v>
       </c>
       <c r="B112">
-        <f t="shared" ca="1" si="5"/>
-        <v>1.756048982538564E-3</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.17526634373256897</v>
       </c>
       <c r="C112" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A112^2+B112^2, 0)  + _c2*BESSELJ(_c3*A112^2+_c4*B112^2, 0)  - _c5*BESSELJ(_c6*A112^2+_c7*B112^2, 0)</f>
-        <v>4.0717144080104521</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.39449437490099931</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A113">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.25539316831081921</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.68340301500594625</v>
       </c>
       <c r="B113">
-        <f t="shared" ca="1" si="5"/>
-        <v>-0.17154841785865693</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.25977233447479703</v>
       </c>
       <c r="C113" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A113^2+B113^2, 0)  + _c2*BESSELJ(_c3*A113^2+_c4*B113^2, 0)  - _c5*BESSELJ(_c6*A113^2+_c7*B113^2, 0)</f>
-        <v>2.9603573481738135</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.0882409244185367</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A114">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.34964990809060859</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.64660710341628713</v>
       </c>
       <c r="B114">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.36458764999283388</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.25818544175703495</v>
       </c>
       <c r="C114" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A114^2+B114^2, 0)  + _c2*BESSELJ(_c3*A114^2+_c4*B114^2, 0)  - _c5*BESSELJ(_c6*A114^2+_c7*B114^2, 0)</f>
-        <v>1.4147882144798478</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.7727236953525907</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A115">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.13415590500504435</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-6.3511950375601131E-2</v>
       </c>
       <c r="B115">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.1457692818060729</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.45775144100895049</v>
       </c>
       <c r="C115" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A115^2+B115^2, 0)  + _c2*BESSELJ(_c3*A115^2+_c4*B115^2, 0)  - _c5*BESSELJ(_c6*A115^2+_c7*B115^2, 0)</f>
-        <v>2.9486862539767147</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>-0.15348921511528313</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A116">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.16416496806105549</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.13387781190923881</v>
       </c>
       <c r="B116">
-        <f t="shared" ca="1" si="5"/>
-        <v>-0.37896935393328629</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.3875375667113013</v>
       </c>
       <c r="C116" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A116^2+B116^2, 0)  + _c2*BESSELJ(_c3*A116^2+_c4*B116^2, 0)  - _c5*BESSELJ(_c6*A116^2+_c7*B116^2, 0)</f>
-        <v>1.1792157690946627</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.0681691369363957</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A117">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.64450058828677348</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.11648125233043996</v>
       </c>
       <c r="B117">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.28194089205839712</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.34800729839021982</v>
       </c>
       <c r="C117" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A117^2+B117^2, 0)  + _c2*BESSELJ(_c3*A117^2+_c4*B117^2, 0)  - _c5*BESSELJ(_c6*A117^2+_c7*B117^2, 0)</f>
-        <v>1.5213501233814055</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.6701856392275991</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A118">
-        <f t="shared" ca="1" si="5"/>
-        <v>-0.12166588465602009</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.28550793810388153</v>
       </c>
       <c r="B118">
-        <f t="shared" ca="1" si="5"/>
-        <v>-7.9683779337267613E-2</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.37463876316317729</v>
       </c>
       <c r="C118" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A118^2+B118^2, 0)  + _c2*BESSELJ(_c3*A118^2+_c4*B118^2, 0)  - _c5*BESSELJ(_c6*A118^2+_c7*B118^2, 0)</f>
-        <v>2.9987783024371457</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.205316738673752</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A119">
-        <f t="shared" ca="1" si="5"/>
-        <v>-0.43732181753335608</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.30178096828234152</v>
       </c>
       <c r="B119">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.28494988222061368</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.40759361026803914</v>
       </c>
       <c r="C119" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A119^2+B119^2, 0)  + _c2*BESSELJ(_c3*A119^2+_c4*B119^2, 0)  - _c5*BESSELJ(_c6*A119^2+_c7*B119^2, 0)</f>
-        <v>2.5857278393880643</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>0.69628092780501794</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A120">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.5753201682351895</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.16666798871511121</v>
       </c>
       <c r="B120">
-        <f t="shared" ca="1" si="5"/>
-        <v>-8.8737670370917773E-2</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0.82810479252679081</v>
       </c>
       <c r="C120" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A120^2+B120^2, 0)  + _c2*BESSELJ(_c3*A120^2+_c4*B120^2, 0)  - _c5*BESSELJ(_c6*A120^2+_c7*B120^2, 0)</f>
-        <v>3.9359634914114863</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.0023956012063473</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A121">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.93721053630112205</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.11428601236334067</v>
       </c>
       <c r="B121">
-        <f t="shared" ca="1" si="5"/>
-        <v>0.26861232858605727</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-0.10023068937779812</v>
       </c>
       <c r="C121" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A121^2+B121^2, 0)  + _c2*BESSELJ(_c3*A121^2+_c4*B121^2, 0)  - _c5*BESSELJ(_c6*A121^2+_c7*B121^2, 0)</f>
-        <v>-0.51871237789298585</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.98948070582792</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A122">
-        <f t="shared" ref="A122:B141" ca="1" si="6">_xlfn.NORM.INV(RAND(),0,0.5)</f>
-        <v>0.62037290870930217</v>
+        <f t="shared" ref="A122:B141" ca="1" si="8">_xlfn.NORM.INV(RAND(),0,0.5)</f>
+        <v>1.0761248784546043</v>
       </c>
       <c r="B122">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.26790161660525624</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.5243273908572389</v>
       </c>
       <c r="C122" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A122^2+B122^2, 0)  + _c2*BESSELJ(_c3*A122^2+_c4*B122^2, 0)  - _c5*BESSELJ(_c6*A122^2+_c7*B122^2, 0)</f>
-        <v>2.0481628639173799</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1.4102656737950374</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A123">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.76407264831644295</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.62209662655080011</v>
       </c>
       <c r="B123">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.55947627133202393</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.45746718307648959</v>
       </c>
       <c r="C123" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A123^2+B123^2, 0)  + _c2*BESSELJ(_c3*A123^2+_c4*B123^2, 0)  - _c5*BESSELJ(_c6*A123^2+_c7*B123^2, 0)</f>
-        <v>0.15096355045326315</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>-2.6122177784100087E-2</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A124">
-        <f t="shared" ca="1" si="6"/>
-        <v>8.6611531681822104E-2</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.28910740938019014</v>
       </c>
       <c r="B124">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.78298617982959551</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.30143492683500439</v>
       </c>
       <c r="C124" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A124^2+B124^2, 0)  + _c2*BESSELJ(_c3*A124^2+_c4*B124^2, 0)  - _c5*BESSELJ(_c6*A124^2+_c7*B124^2, 0)</f>
-        <v>1.1285225305076889</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.1590878679467629</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A125">
-        <f t="shared" ca="1" si="6"/>
-        <v>-0.84071447497938667</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.50520673522680615</v>
       </c>
       <c r="B125">
-        <f t="shared" ca="1" si="6"/>
-        <v>-0.16737679123995822</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.31554599482257578</v>
       </c>
       <c r="C125" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A125^2+B125^2, 0)  + _c2*BESSELJ(_c3*A125^2+_c4*B125^2, 0)  - _c5*BESSELJ(_c6*A125^2+_c7*B125^2, 0)</f>
-        <v>-0.90225382355367889</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2.2370424879134077</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A126">
-        <f t="shared" ca="1" si="6"/>
-        <v>-6.7088946417305589E-2</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.40665144875230397</v>
       </c>
       <c r="B126">
-        <f t="shared" ca="1" si="6"/>
-        <v>4.0979557680801505E-2</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.14824681918461699</v>
       </c>
       <c r="C126" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A126^2+B126^2, 0)  + _c2*BESSELJ(_c3*A126^2+_c4*B126^2, 0)  - _c5*BESSELJ(_c6*A126^2+_c7*B126^2, 0)</f>
-        <v>3.0000318907192387</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>3.4782448642215007</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A127">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.23112578563193714</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.10295289013784241</v>
       </c>
       <c r="B127">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.30303804835343862</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.53148663144189168</v>
       </c>
       <c r="C127" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A127^2+B127^2, 0)  + _c2*BESSELJ(_c3*A127^2+_c4*B127^2, 0)  - _c5*BESSELJ(_c6*A127^2+_c7*B127^2, 0)</f>
-        <v>2.1269688123948844</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>-1.4392258869977106</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A128">
-        <f t="shared" ca="1" si="6"/>
-        <v>-0.53226442048295608</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.65279628200348028</v>
       </c>
       <c r="B128">
-        <f t="shared" ca="1" si="6"/>
-        <v>-1.0926955202447224E-3</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.52119539372326174</v>
       </c>
       <c r="C128" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A128^2+B128^2, 0)  + _c2*BESSELJ(_c3*A128^2+_c4*B128^2, 0)  - _c5*BESSELJ(_c6*A128^2+_c7*B128^2, 0)</f>
-        <v>4.192083489820992</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>-0.16523163164553611</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A129">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.10875629580633095</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-1.182723346912439E-2</v>
       </c>
       <c r="B129">
-        <f t="shared" ca="1" si="6"/>
-        <v>-0.56353645488829363</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.57995713961904938</v>
       </c>
       <c r="C129" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A129^2+B129^2, 0)  + _c2*BESSELJ(_c3*A129^2+_c4*B129^2, 0)  - _c5*BESSELJ(_c6*A129^2+_c7*B129^2, 0)</f>
-        <v>-1.7976675852162645</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>-1.9796127365023557</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A130">
-        <f t="shared" ca="1" si="6"/>
-        <v>-0.16127097714498428</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>8.5109129099300046E-2</v>
       </c>
       <c r="B130">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.49789067510697621</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.73454099448816457</v>
       </c>
       <c r="C130" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A130^2+B130^2, 0)  + _c2*BESSELJ(_c3*A130^2+_c4*B130^2, 0)  - _c5*BESSELJ(_c6*A130^2+_c7*B130^2, 0)</f>
-        <v>-0.90075711903187428</v>
+        <f t="shared" ref="C130:C193" ca="1" si="9" xml:space="preserve"> _c1*BESSELJ(A130^2+B130^2, 0)  + _c2*BESSELJ(_c3*A130^2+_c4*B130^2, 0)  - _c5*BESSELJ(_c6*A130^2+_c7*B130^2, 0)</f>
+        <v>-1.0681040890292981E-2</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A131">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.33639196535778942</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.28765343815046018</v>
       </c>
       <c r="B131">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.25826594586321844</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.17131280866118448</v>
       </c>
       <c r="C131" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A131^2+B131^2, 0)  + _c2*BESSELJ(_c3*A131^2+_c4*B131^2, 0)  - _c5*BESSELJ(_c6*A131^2+_c7*B131^2, 0)</f>
-        <v>2.6263175668187269</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>3.0139271948418154</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A132">
-        <f t="shared" ca="1" si="6"/>
-        <v>-9.7681829084974914E-2</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.34369867002218957</v>
       </c>
       <c r="B132">
-        <f t="shared" ca="1" si="6"/>
-        <v>-0.28889175245930598</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.36603347098638123</v>
       </c>
       <c r="C132" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A132^2+B132^2, 0)  + _c2*BESSELJ(_c3*A132^2+_c4*B132^2, 0)  - _c5*BESSELJ(_c6*A132^2+_c7*B132^2, 0)</f>
-        <v>2.3309879182012097</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>1.3855658929598647</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A133">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.63666218829539611</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.15852523225701326</v>
       </c>
       <c r="B133">
-        <f t="shared" ca="1" si="6"/>
-        <v>-8.7163243510621158E-2</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>9.0950348419963269E-3</v>
       </c>
       <c r="C133" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A133^2+B133^2, 0)  + _c2*BESSELJ(_c3*A133^2+_c4*B133^2, 0)  - _c5*BESSELJ(_c6*A133^2+_c7*B133^2, 0)</f>
-        <v>3.3379861829628288</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>3.0210901857234029</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A134">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.11511459712743559</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.23168612136010178</v>
       </c>
       <c r="B134">
-        <f t="shared" ca="1" si="6"/>
-        <v>-0.39334678502329196</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.39920619312838729</v>
       </c>
       <c r="C134" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A134^2+B134^2, 0)  + _c2*BESSELJ(_c3*A134^2+_c4*B134^2, 0)  - _c5*BESSELJ(_c6*A134^2+_c7*B134^2, 0)</f>
-        <v>0.98815101765830016</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0.81193357029832813</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A135">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.71837159445651599</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>8.4068382758454741E-2</v>
       </c>
       <c r="B135">
-        <f t="shared" ca="1" si="6"/>
-        <v>-0.87264909566841964</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.28286190926261379</v>
       </c>
       <c r="C135" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A135^2+B135^2, 0)  + _c2*BESSELJ(_c3*A135^2+_c4*B135^2, 0)  - _c5*BESSELJ(_c6*A135^2+_c7*B135^2, 0)</f>
-        <v>-0.7923993628351601</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.3887486291128499</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A136">
-        <f t="shared" ca="1" si="6"/>
-        <v>-5.8519454452371084E-2</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.15546548159276735</v>
       </c>
       <c r="B136">
-        <f t="shared" ca="1" si="6"/>
-        <v>-0.14652898787236734</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.69114775150269692</v>
       </c>
       <c r="C136" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A136^2+B136^2, 0)  + _c2*BESSELJ(_c3*A136^2+_c4*B136^2, 0)  - _c5*BESSELJ(_c6*A136^2+_c7*B136^2, 0)</f>
-        <v>2.9527095195473034</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>-0.75915191937344073</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A137">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.71931451628679699</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.61054383752471642</v>
       </c>
       <c r="B137">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.91887939677313535</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.15428149690537274</v>
       </c>
       <c r="C137" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A137^2+B137^2, 0)  + _c2*BESSELJ(_c3*A137^2+_c4*B137^2, 0)  - _c5*BESSELJ(_c6*A137^2+_c7*B137^2, 0)</f>
-        <v>-0.82146599709323853</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>3.2907919831694352</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A138">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.52312868217252373</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.18730044520253034</v>
       </c>
       <c r="B138">
-        <f t="shared" ca="1" si="6"/>
-        <v>4.592624689111463E-2</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-8.9308277096792302E-2</v>
       </c>
       <c r="C138" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A138^2+B138^2, 0)  + _c2*BESSELJ(_c3*A138^2+_c4*B138^2, 0)  - _c5*BESSELJ(_c6*A138^2+_c7*B138^2, 0)</f>
-        <v>4.1520340010220007</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>3.0208474602684143</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A139">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.19926868319915228</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.31206623772027303</v>
       </c>
       <c r="B139">
-        <f t="shared" ca="1" si="6"/>
-        <v>-6.4397772231448824E-2</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.74955533300095856</v>
       </c>
       <c r="C139" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A139^2+B139^2, 0)  + _c2*BESSELJ(_c3*A139^2+_c4*B139^2, 0)  - _c5*BESSELJ(_c6*A139^2+_c7*B139^2, 0)</f>
-        <v>3.0424775470070675</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>1.7540430259110302</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A140">
-        <f t="shared" ca="1" si="6"/>
-        <v>-0.45289706049418943</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-0.2699459345828118</v>
       </c>
       <c r="B140">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.20300152258837073</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-7.5064929896401969E-2</v>
       </c>
       <c r="C140" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A140^2+B140^2, 0)  + _c2*BESSELJ(_c3*A140^2+_c4*B140^2, 0)  - _c5*BESSELJ(_c6*A140^2+_c7*B140^2, 0)</f>
-        <v>3.355140979369414</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>3.1468438194825579</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A141">
-        <f t="shared" ca="1" si="6"/>
-        <v>0.23890359929214366</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>-5.9367957106353952E-2</v>
       </c>
       <c r="B141">
-        <f t="shared" ca="1" si="6"/>
-        <v>-0.21051909945707706</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.79715152663545163</v>
       </c>
       <c r="C141" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A141^2+B141^2, 0)  + _c2*BESSELJ(_c3*A141^2+_c4*B141^2, 0)  - _c5*BESSELJ(_c6*A141^2+_c7*B141^2, 0)</f>
-        <v>2.7991320299800764</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>1.3350622477195211</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A142">
-        <f t="shared" ref="A142:B161" ca="1" si="7">_xlfn.NORM.INV(RAND(),0,0.5)</f>
-        <v>0.25910831089004455</v>
+        <f t="shared" ref="A142:B161" ca="1" si="10">_xlfn.NORM.INV(RAND(),0,0.5)</f>
+        <v>-1.1714446286210453E-2</v>
       </c>
       <c r="B142">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.75816165206383435</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>0.29343524804478499</v>
       </c>
       <c r="C142" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A142^2+B142^2, 0)  + _c2*BESSELJ(_c3*A142^2+_c4*B142^2, 0)  - _c5*BESSELJ(_c6*A142^2+_c7*B142^2, 0)</f>
-        <v>1.5110959820004253</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.3231178185632251</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A143">
-        <f t="shared" ca="1" si="7"/>
-        <v>-6.8113502054124406E-2</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>0.62156281193103002</v>
       </c>
       <c r="B143">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.74831920685009801</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.97240376430854292</v>
       </c>
       <c r="C143" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A143^2+B143^2, 0)  + _c2*BESSELJ(_c3*A143^2+_c4*B143^2, 0)  - _c5*BESSELJ(_c6*A143^2+_c7*B143^2, 0)</f>
-        <v>0.28877490512100068</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>-0.65084805470685647</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A144">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.36840706002164514</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.38758142495069509</v>
       </c>
       <c r="B144">
-        <f t="shared" ca="1" si="7"/>
-        <v>8.5987074162121313E-2</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>8.6366894670687214E-2</v>
       </c>
       <c r="C144" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A144^2+B144^2, 0)  + _c2*BESSELJ(_c3*A144^2+_c4*B144^2, 0)  - _c5*BESSELJ(_c6*A144^2+_c7*B144^2, 0)</f>
-        <v>3.4674153892354158</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>3.5542271598237223</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A145">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.63466780338889039</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.29884126043086096</v>
       </c>
       <c r="B145">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.33937412176142262</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.25757083585608015</v>
       </c>
       <c r="C145" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A145^2+B145^2, 0)  + _c2*BESSELJ(_c3*A145^2+_c4*B145^2, 0)  - _c5*BESSELJ(_c6*A145^2+_c7*B145^2, 0)</f>
-        <v>0.95052818132514494</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.571440407957196</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A146">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.54531361261934175</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>0.27056605404873868</v>
       </c>
       <c r="B146">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.3920812280905886</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>0.90989110210988788</v>
       </c>
       <c r="C146" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A146^2+B146^2, 0)  + _c2*BESSELJ(_c3*A146^2+_c4*B146^2, 0)  - _c5*BESSELJ(_c6*A146^2+_c7*B146^2, 0)</f>
-        <v>1.0737505629214175</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>1.5448263863849008</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A147">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.10620316833690782</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.31722869650410185</v>
       </c>
       <c r="B147">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.13765450827637271</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.12721426293684079</v>
       </c>
       <c r="C147" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A147^2+B147^2, 0)  + _c2*BESSELJ(_c3*A147^2+_c4*B147^2, 0)  - _c5*BESSELJ(_c6*A147^2+_c7*B147^2, 0)</f>
-        <v>2.9592841217392558</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>3.203237463545193</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A148">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.36701166686060949</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-1.1432201046147312</v>
       </c>
       <c r="B148">
-        <f t="shared" ca="1" si="7"/>
-        <v>-5.6684270654049122E-2</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.2614415521579414</v>
       </c>
       <c r="C148" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A148^2+B148^2, 0)  + _c2*BESSELJ(_c3*A148^2+_c4*B148^2, 0)  - _c5*BESSELJ(_c6*A148^2+_c7*B148^2, 0)</f>
-        <v>3.4954940354129418</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0.64545158463828256</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A149">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.13316651177111199</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.56531096414386506</v>
       </c>
       <c r="B149">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.24357071365954938</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-1.3609790545049401</v>
       </c>
       <c r="C149" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A149^2+B149^2, 0)  + _c2*BESSELJ(_c3*A149^2+_c4*B149^2, 0)  - _c5*BESSELJ(_c6*A149^2+_c7*B149^2, 0)</f>
-        <v>2.6319974507471375</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0.8873268628648171</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A150">
-        <f t="shared" ca="1" si="7"/>
-        <v>-5.4621842694934294E-2</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.99581552456934941</v>
       </c>
       <c r="B150">
-        <f t="shared" ca="1" si="7"/>
-        <v>8.6831642922446661E-3</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>4.607285322942322E-2</v>
       </c>
       <c r="C150" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A150^2+B150^2, 0)  + _c2*BESSELJ(_c3*A150^2+_c4*B150^2, 0)  - _c5*BESSELJ(_c6*A150^2+_c7*B150^2, 0)</f>
-        <v>3.0002885073892176</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>-0.34009316993094296</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A151">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.50858501165614156</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.73966960795186332</v>
       </c>
       <c r="B151">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.26602929644326923</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>0.79432678738909723</v>
       </c>
       <c r="C151" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A151^2+B151^2, 0)  + _c2*BESSELJ(_c3*A151^2+_c4*B151^2, 0)  - _c5*BESSELJ(_c6*A151^2+_c7*B151^2, 0)</f>
-        <v>2.8361009768152337</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0.28720119719592208</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A152">
-        <f t="shared" ca="1" si="7"/>
-        <v>-1.3175572230711918E-2</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>0.17005102563715505</v>
       </c>
       <c r="B152">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.47841633849615883</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.38579349789265904</v>
       </c>
       <c r="C152" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A152^2+B152^2, 0)  + _c2*BESSELJ(_c3*A152^2+_c4*B152^2, 0)  - _c5*BESSELJ(_c6*A152^2+_c7*B152^2, 0)</f>
-        <v>-0.5382263498983022</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>1.0661197862291545</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A153">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.12538396808284027</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>0.21271610517184453</v>
       </c>
       <c r="B153">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.20137253864697441</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>0.2715311792726196</v>
       </c>
       <c r="C153" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A153^2+B153^2, 0)  + _c2*BESSELJ(_c3*A153^2+_c4*B153^2, 0)  - _c5*BESSELJ(_c6*A153^2+_c7*B153^2, 0)</f>
-        <v>2.8215000666716783</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.4171913573809132</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A154">
-        <f t="shared" ca="1" si="7"/>
-        <v>4.9296080547377129E-3</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.21781921122293368</v>
       </c>
       <c r="B154">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.58980035839320533</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>6.6460999308132929E-2</v>
       </c>
       <c r="C154" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A154^2+B154^2, 0)  + _c2*BESSELJ(_c3*A154^2+_c4*B154^2, 0)  - _c5*BESSELJ(_c6*A154^2+_c7*B154^2, 0)</f>
-        <v>-2.0296782325334308</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>3.0619522759553868</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A155">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.2934845538270171</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-7.2672676139532585E-2</v>
       </c>
       <c r="B155">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.14573693283359695</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.45238354874227349</v>
       </c>
       <c r="C155" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A155^2+B155^2, 0)  + _c2*BESSELJ(_c3*A155^2+_c4*B155^2, 0)  - _c5*BESSELJ(_c6*A155^2+_c7*B155^2, 0)</f>
-        <v>3.0984274784657373</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>-5.458968271750031E-2</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A156">
-        <f t="shared" ca="1" si="7"/>
-        <v>-1.107879199496252</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-1.0795681760263636</v>
       </c>
       <c r="B156">
-        <f t="shared" ca="1" si="7"/>
-        <v>-5.9181254412929374E-2</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>0.27076205063980413</v>
       </c>
       <c r="C156" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A156^2+B156^2, 0)  + _c2*BESSELJ(_c3*A156^2+_c4*B156^2, 0)  - _c5*BESSELJ(_c6*A156^2+_c7*B156^2, 0)</f>
-        <v>-0.34215656033522251</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0.44141505599674041</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A157">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.5520483690325606</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>0.20910504812889461</v>
       </c>
       <c r="B157">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.38927815041665637</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.27211090724723858</v>
       </c>
       <c r="C157" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A157^2+B157^2, 0)  + _c2*BESSELJ(_c3*A157^2+_c4*B157^2, 0)  - _c5*BESSELJ(_c6*A157^2+_c7*B157^2, 0)</f>
-        <v>1.079638415149029</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.4131054191494687</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A158">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.6823617741815251</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.67570511668854649</v>
       </c>
       <c r="B158">
-        <f t="shared" ca="1" si="7"/>
-        <v>-6.4471234297733437E-2</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.23890776572545899</v>
       </c>
       <c r="C158" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A158^2+B158^2, 0)  + _c2*BESSELJ(_c3*A158^2+_c4*B158^2, 0)  - _c5*BESSELJ(_c6*A158^2+_c7*B158^2, 0)</f>
-        <v>2.6194306506452794</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>1.4689568576321128</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A159">
-        <f t="shared" ca="1" si="7"/>
-        <v>-5.6013067218584268E-2</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>0.21227873753476811</v>
       </c>
       <c r="B159">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.39579753805887535</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>7.740276884684634E-2</v>
       </c>
       <c r="C159" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A159^2+B159^2, 0)  + _c2*BESSELJ(_c3*A159^2+_c4*B159^2, 0)  - _c5*BESSELJ(_c6*A159^2+_c7*B159^2, 0)</f>
-        <v>0.98648546812831173</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>3.0501724020111043</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A160">
-        <f t="shared" ca="1" si="7"/>
-        <v>-2.4823568899470076E-2</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-0.22163594241269724</v>
       </c>
       <c r="B160">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.19473229002587278</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>0.40912619014093504</v>
       </c>
       <c r="C160" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A160^2+B160^2, 0)  + _c2*BESSELJ(_c3*A160^2+_c4*B160^2, 0)  - _c5*BESSELJ(_c6*A160^2+_c7*B160^2, 0)</f>
-        <v>2.86246100987012</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0.6483817922023758</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A161">
-        <f t="shared" ca="1" si="7"/>
-        <v>-0.60886902771751716</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>0.66290380932380699</v>
       </c>
       <c r="B161">
-        <f t="shared" ca="1" si="7"/>
-        <v>-1.3303434318067979</v>
+        <f t="shared" ca="1" si="10"/>
+        <v>-6.4871769568394674E-2</v>
       </c>
       <c r="C161" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A161^2+B161^2, 0)  + _c2*BESSELJ(_c3*A161^2+_c4*B161^2, 0)  - _c5*BESSELJ(_c6*A161^2+_c7*B161^2, 0)</f>
-        <v>0.98519096039246712</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.9933358990554026</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A162">
-        <f t="shared" ref="A162:B181" ca="1" si="8">_xlfn.NORM.INV(RAND(),0,0.5)</f>
-        <v>0.49728245128576476</v>
+        <f t="shared" ref="A162:B181" ca="1" si="11">_xlfn.NORM.INV(RAND(),0,0.5)</f>
+        <v>-0.28752529703064628</v>
       </c>
       <c r="B162">
-        <f t="shared" ca="1" si="8"/>
-        <v>-0.82955054339839485</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.58655921899834051</v>
       </c>
       <c r="C162" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A162^2+B162^2, 0)  + _c2*BESSELJ(_c3*A162^2+_c4*B162^2, 0)  - _c5*BESSELJ(_c6*A162^2+_c7*B162^2, 0)</f>
-        <v>2.2192075521424721</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>-1.2645637185450549</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A163">
-        <f t="shared" ca="1" si="8"/>
-        <v>-0.31763528905727134</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.35085188590837907</v>
       </c>
       <c r="B163">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.2464301823229435</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.27304246666293186</v>
       </c>
       <c r="C163" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A163^2+B163^2, 0)  + _c2*BESSELJ(_c3*A163^2+_c4*B163^2, 0)  - _c5*BESSELJ(_c6*A163^2+_c7*B163^2, 0)</f>
-        <v>2.6839924435180862</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.5245202623792258</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A164">
-        <f t="shared" ca="1" si="8"/>
-        <v>-0.59775670715936857</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>9.0031007281585265E-2</v>
       </c>
       <c r="B164">
-        <f t="shared" ca="1" si="8"/>
-        <v>1.8114362022090408E-2</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.27519680722344697</v>
       </c>
       <c r="C164" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A164^2+B164^2, 0)  + _c2*BESSELJ(_c3*A164^2+_c4*B164^2, 0)  - _c5*BESSELJ(_c6*A164^2+_c7*B164^2, 0)</f>
-        <v>3.9431161944013811</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.445656153523978</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A165">
-        <f t="shared" ca="1" si="8"/>
-        <v>-0.7544641893475631</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.20649676129078118</v>
       </c>
       <c r="B165">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.26360116851173515</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.37680663006238108</v>
       </c>
       <c r="C165" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A165^2+B165^2, 0)  + _c2*BESSELJ(_c3*A165^2+_c4*B165^2, 0)  - _c5*BESSELJ(_c6*A165^2+_c7*B165^2, 0)</f>
-        <v>-0.34510629659815839</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>1.1820722290840247</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A166">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.39885729385474694</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.41796365123303303</v>
       </c>
       <c r="B166">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.32686582216676185</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.57072102938498226</v>
       </c>
       <c r="C166" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A166^2+B166^2, 0)  + _c2*BESSELJ(_c3*A166^2+_c4*B166^2, 0)  - _c5*BESSELJ(_c6*A166^2+_c7*B166^2, 0)</f>
-        <v>2.0129362376602211</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>-0.35436334965112443</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A167">
-        <f t="shared" ca="1" si="8"/>
-        <v>-0.65974859335493963</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.6889982601089959</v>
       </c>
       <c r="B167">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.1008578542635751</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.36018092931392437</v>
       </c>
       <c r="C167" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A167^2+B167^2, 0)  + _c2*BESSELJ(_c3*A167^2+_c4*B167^2, 0)  - _c5*BESSELJ(_c6*A167^2+_c7*B167^2, 0)</f>
-        <v>2.9026096965418144</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>-0.10197357777688515</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A168">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.43420746211768485</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.70028829914868262</v>
       </c>
       <c r="B168">
-        <f t="shared" ca="1" si="8"/>
-        <v>-0.49390386093496474</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-9.1864257741181912E-2</v>
       </c>
       <c r="C168" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A168^2+B168^2, 0)  + _c2*BESSELJ(_c3*A168^2+_c4*B168^2, 0)  - _c5*BESSELJ(_c6*A168^2+_c7*B168^2, 0)</f>
-        <v>-0.11048825334628537</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.1293612871303305</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A169">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.15268498325425073</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.34924259772331634</v>
       </c>
       <c r="B169">
-        <f t="shared" ca="1" si="8"/>
-        <v>1.2040481248079736E-2</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.22135657957520669</v>
       </c>
       <c r="C169" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A169^2+B169^2, 0)  + _c2*BESSELJ(_c3*A169^2+_c4*B169^2, 0)  - _c5*BESSELJ(_c6*A169^2+_c7*B169^2, 0)</f>
-        <v>3.0180820208992367</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.9225311371371214</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A170">
-        <f t="shared" ca="1" si="8"/>
-        <v>-0.26774211399073233</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.23924240065351982</v>
       </c>
       <c r="B170">
-        <f t="shared" ca="1" si="8"/>
-        <v>-0.62872791885126988</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.12407271073389327</v>
       </c>
       <c r="C170" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A170^2+B170^2, 0)  + _c2*BESSELJ(_c3*A170^2+_c4*B170^2, 0)  - _c5*BESSELJ(_c6*A170^2+_c7*B170^2, 0)</f>
-        <v>-1.0973335350841547</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>3.0401928031307524</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A171">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.63858978765644125</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.11690295965131922</v>
       </c>
       <c r="B171">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.30496841183888174</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.51290451145424276</v>
       </c>
       <c r="C171" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A171^2+B171^2, 0)  + _c2*BESSELJ(_c3*A171^2+_c4*B171^2, 0)  - _c5*BESSELJ(_c6*A171^2+_c7*B171^2, 0)</f>
-        <v>1.3262678973631505</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>-1.1566907938805842</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A172">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.1252480170130299</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.37775282964808427</v>
       </c>
       <c r="B172">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.8018179541300906</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.30399054403211101</v>
       </c>
       <c r="C172" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A172^2+B172^2, 0)  + _c2*BESSELJ(_c3*A172^2+_c4*B172^2, 0)  - _c5*BESSELJ(_c6*A172^2+_c7*B172^2, 0)</f>
-        <v>1.5802092055356951</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.2538211452661709</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A173">
-        <f t="shared" ca="1" si="8"/>
-        <v>-0.16368724015736374</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.13877323521044535</v>
       </c>
       <c r="B173">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.7272764407436344</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.16958859906209992</v>
       </c>
       <c r="C173" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A173^2+B173^2, 0)  + _c2*BESSELJ(_c3*A173^2+_c4*B173^2, 0)  - _c5*BESSELJ(_c6*A173^2+_c7*B173^2, 0)</f>
-        <v>0.13827869721536978</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.9062589470159632</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A174">
-        <f t="shared" ca="1" si="8"/>
-        <v>-0.49975451430754941</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.16921917822706573</v>
       </c>
       <c r="B174">
-        <f t="shared" ca="1" si="8"/>
-        <v>-1.6774272669416966E-2</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.46411381584382494</v>
       </c>
       <c r="C174" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A174^2+B174^2, 0)  + _c2*BESSELJ(_c3*A174^2+_c4*B174^2, 0)  - _c5*BESSELJ(_c6*A174^2+_c7*B174^2, 0)</f>
-        <v>4.1371613719089844</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>-0.31266693596852169</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A175">
-        <f t="shared" ca="1" si="8"/>
-        <v>1.0593549720309439</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.36560234398958202</v>
       </c>
       <c r="B175">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.3299319057965821</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.45073237987661841</v>
       </c>
       <c r="C175" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A175^2+B175^2, 0)  + _c2*BESSELJ(_c3*A175^2+_c4*B175^2, 0)  - _c5*BESSELJ(_c6*A175^2+_c7*B175^2, 0)</f>
-        <v>0.84607429069724716</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0.13870594534043235</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A176">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.36154798266075738</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.35720998829103079</v>
       </c>
       <c r="B176">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.33544190028593185</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-8.6731427501606978E-2</v>
       </c>
       <c r="C176" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A176^2+B176^2, 0)  + _c2*BESSELJ(_c3*A176^2+_c4*B176^2, 0)  - _c5*BESSELJ(_c6*A176^2+_c7*B176^2, 0)</f>
-        <v>1.8372088411703555</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>3.4180937443268489</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A177">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.5819810236798767</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>1.24852955318116E-2</v>
       </c>
       <c r="B177">
-        <f t="shared" ca="1" si="8"/>
-        <v>-6.1050064372855158E-2</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>0.1375779306011933</v>
       </c>
       <c r="C177" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A177^2+B177^2, 0)  + _c2*BESSELJ(_c3*A177^2+_c4*B177^2, 0)  - _c5*BESSELJ(_c6*A177^2+_c7*B177^2, 0)</f>
-        <v>3.9834139213426303</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.9656295256219316</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A178">
-        <f t="shared" ca="1" si="8"/>
-        <v>-5.8260088927174448E-3</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.48904446962782061</v>
       </c>
       <c r="B178">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.22858732579639407</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.59414333506348527</v>
       </c>
       <c r="C178" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A178^2+B178^2, 0)  + _c2*BESSELJ(_c3*A178^2+_c4*B178^2, 0)  - _c5*BESSELJ(_c6*A178^2+_c7*B178^2, 0)</f>
-        <v>2.7430950686664222</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0.36556826535029852</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A179">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.20464981921736158</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.73282419381990205</v>
       </c>
       <c r="B179">
-        <f t="shared" ca="1" si="8"/>
-        <v>-0.58792222023426111</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.2370288208972445</v>
       </c>
       <c r="C179" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A179^2+B179^2, 0)  + _c2*BESSELJ(_c3*A179^2+_c4*B179^2, 0)  - _c5*BESSELJ(_c6*A179^2+_c7*B179^2, 0)</f>
-        <v>-1.6856931296544584</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0.31386492818856776</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A180">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.31711256021152484</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.83592992740213334</v>
       </c>
       <c r="B180">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.78931624933498323</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-9.530469273296964E-2</v>
       </c>
       <c r="C180" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A180^2+B180^2, 0)  + _c2*BESSELJ(_c3*A180^2+_c4*B180^2, 0)  - _c5*BESSELJ(_c6*A180^2+_c7*B180^2, 0)</f>
-        <v>2.4144766990922149</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>-0.59763034161033102</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A181">
-        <f t="shared" ca="1" si="8"/>
-        <v>6.504500263564697E-2</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.42396200831841613</v>
       </c>
       <c r="B181">
-        <f t="shared" ca="1" si="8"/>
-        <v>0.50577633940690225</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>-0.84165518274206252</v>
       </c>
       <c r="C181" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A181^2+B181^2, 0)  + _c2*BESSELJ(_c3*A181^2+_c4*B181^2, 0)  - _c5*BESSELJ(_c6*A181^2+_c7*B181^2, 0)</f>
-        <v>-1.0420217259084161</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.4739039255207023</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A182">
-        <f t="shared" ref="A182:B201" ca="1" si="9">_xlfn.NORM.INV(RAND(),0,0.5)</f>
-        <v>-0.47447177504171784</v>
+        <f t="shared" ref="A182:B201" ca="1" si="12">_xlfn.NORM.INV(RAND(),0,0.5)</f>
+        <v>-0.27870376564824551</v>
       </c>
       <c r="B182">
-        <f t="shared" ca="1" si="9"/>
-        <v>-0.82126934333154933</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-0.25982027768491306</v>
       </c>
       <c r="C182" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A182^2+B182^2, 0)  + _c2*BESSELJ(_c3*A182^2+_c4*B182^2, 0)  - _c5*BESSELJ(_c6*A182^2+_c7*B182^2, 0)</f>
-        <v>2.5148062743911832</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.5319528738793906</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A183">
-        <f t="shared" ca="1" si="9"/>
-        <v>-2.2334251823768546E-2</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.26692398278785046</v>
       </c>
       <c r="B183">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.7635174260156405E-2</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-1.2520238201849998E-2</v>
       </c>
       <c r="C183" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A183^2+B183^2, 0)  + _c2*BESSELJ(_c3*A183^2+_c4*B183^2, 0)  - _c5*BESSELJ(_c6*A183^2+_c7*B183^2, 0)</f>
-        <v>2.9999333232543401</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>3.1632198421625519</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A184">
-        <f t="shared" ca="1" si="9"/>
-        <v>-0.69994261616050968</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-0.29370835037127219</v>
       </c>
       <c r="B184">
-        <f t="shared" ca="1" si="9"/>
-        <v>-0.80483146807113348</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-0.43749737174687198</v>
       </c>
       <c r="C184" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A184^2+B184^2, 0)  + _c2*BESSELJ(_c3*A184^2+_c4*B184^2, 0)  - _c5*BESSELJ(_c6*A184^2+_c7*B184^2, 0)</f>
-        <v>0.34672076542052155</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0.19836501101238269</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A185">
-        <f t="shared" ca="1" si="9"/>
-        <v>-0.80307259877699211</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-8.6927052574885963E-2</v>
       </c>
       <c r="B185">
-        <f t="shared" ca="1" si="9"/>
-        <v>-2.0999607685112512E-2</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-0.22686002363587568</v>
       </c>
       <c r="C185" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A185^2+B185^2, 0)  + _c2*BESSELJ(_c3*A185^2+_c4*B185^2, 0)  - _c5*BESSELJ(_c6*A185^2+_c7*B185^2, 0)</f>
-        <v>3.7100943641454553E-2</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.7340524746959591</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A186">
-        <f t="shared" ca="1" si="9"/>
-        <v>-0.30241564001980836</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-0.70462241086071375</v>
       </c>
       <c r="B186">
-        <f t="shared" ca="1" si="9"/>
-        <v>-0.60496773546160931</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-0.43675651950010558</v>
       </c>
       <c r="C186" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A186^2+B186^2, 0)  + _c2*BESSELJ(_c3*A186^2+_c4*B186^2, 0)  - _c5*BESSELJ(_c6*A186^2+_c7*B186^2, 0)</f>
-        <v>-1.0663099496138031</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>-0.73424406813672849</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A187">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.0566151690053374</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.23876748262025321</v>
       </c>
       <c r="B187">
-        <f t="shared" ca="1" si="9"/>
-        <v>-8.1020171958410256E-2</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.79369954960726719</v>
       </c>
       <c r="C187" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A187^2+B187^2, 0)  + _c2*BESSELJ(_c3*A187^2+_c4*B187^2, 0)  - _c5*BESSELJ(_c6*A187^2+_c7*B187^2, 0)</f>
-        <v>-0.27146540442262757</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>1.998985962663175</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A188">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.96916201539621927</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-0.26505229601175206</v>
       </c>
       <c r="B188">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.27062713049260745</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-1.087892878215369</v>
       </c>
       <c r="C188" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A188^2+B188^2, 0)  + _c2*BESSELJ(_c3*A188^2+_c4*B188^2, 0)  - _c5*BESSELJ(_c6*A188^2+_c7*B188^2, 0)</f>
-        <v>-0.11075656883455404</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>1.6739596210020469</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A189">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.69370168225106388</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-2.9187988663368612E-2</v>
       </c>
       <c r="B189">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.49543770972619078</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>4.3352140868899249E-2</v>
       </c>
       <c r="C189" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A189^2+B189^2, 0)  + _c2*BESSELJ(_c3*A189^2+_c4*B189^2, 0)  - _c5*BESSELJ(_c6*A189^2+_c7*B189^2, 0)</f>
-        <v>-0.5325023428961031</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.99960545480047</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A190">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.12853467878045532</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-1.2350552561237791</v>
       </c>
       <c r="B190">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.31244589320800858</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.39111799195553609</v>
       </c>
       <c r="C190" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A190^2+B190^2, 0)  + _c2*BESSELJ(_c3*A190^2+_c4*B190^2, 0)  - _c5*BESSELJ(_c6*A190^2+_c7*B190^2, 0)</f>
-        <v>2.0854664214170207</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>1.6802263235819102</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A191">
-        <f t="shared" ca="1" si="9"/>
-        <v>-0.49410546049569615</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-1.0428550125552156</v>
       </c>
       <c r="B191">
-        <f t="shared" ca="1" si="9"/>
-        <v>-0.73834934560667509</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.29948341788303756</v>
       </c>
       <c r="C191" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A191^2+B191^2, 0)  + _c2*BESSELJ(_c3*A191^2+_c4*B191^2, 0)  - _c5*BESSELJ(_c6*A191^2+_c7*B191^2, 0)</f>
-        <v>2.6253993376493394</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>0.59429964267265489</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A192">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.97417713618295521</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-0.28730210963467329</v>
       </c>
       <c r="B192">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.5050917601507281</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.16929959777841952</v>
       </c>
       <c r="C192" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A192^2+B192^2, 0)  + _c2*BESSELJ(_c3*A192^2+_c4*B192^2, 0)  - _c5*BESSELJ(_c6*A192^2+_c7*B192^2, 0)</f>
-        <v>2.1002277409545078</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>3.0196912386423347</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A193">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.51398677834630047</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>6.5408364339888073E-2</v>
       </c>
       <c r="B193">
-        <f t="shared" ca="1" si="9"/>
-        <v>-6.6982023366044932E-2</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-6.6471696874287986E-2</v>
       </c>
       <c r="C193" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A193^2+B193^2, 0)  + _c2*BESSELJ(_c3*A193^2+_c4*B193^2, 0)  - _c5*BESSELJ(_c6*A193^2+_c7*B193^2, 0)</f>
-        <v>4.1023182065946733</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>2.9977943728139076</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A194">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.73319346427716048</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.49931851902991881</v>
       </c>
       <c r="B194">
-        <f t="shared" ca="1" si="9"/>
-        <v>-0.39321049895361587</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.38394539207059086</v>
       </c>
       <c r="C194" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A194^2+B194^2, 0)  + _c2*BESSELJ(_c3*A194^2+_c4*B194^2, 0)  - _c5*BESSELJ(_c6*A194^2+_c7*B194^2, 0)</f>
-        <v>-0.92017071347998902</v>
+        <f t="shared" ref="C194:C257" ca="1" si="13" xml:space="preserve"> _c1*BESSELJ(A194^2+B194^2, 0)  + _c2*BESSELJ(_c3*A194^2+_c4*B194^2, 0)  - _c5*BESSELJ(_c6*A194^2+_c7*B194^2, 0)</f>
+        <v>1.2995148345109941</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A195">
-        <f t="shared" ca="1" si="9"/>
-        <v>-5.0697217274425825E-2</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-0.58911629634044838</v>
       </c>
       <c r="B195">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.54321505897391698</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-0.28452616253155721</v>
       </c>
       <c r="C195" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A195^2+B195^2, 0)  + _c2*BESSELJ(_c3*A195^2+_c4*B195^2, 0)  - _c5*BESSELJ(_c6*A195^2+_c7*B195^2, 0)</f>
-        <v>-1.614479653145581</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>2.2009360458178429</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A196">
-        <f t="shared" ca="1" si="9"/>
-        <v>-0.44622196597235103</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>3.0999502732021476E-2</v>
       </c>
       <c r="B196">
-        <f t="shared" ca="1" si="9"/>
-        <v>-0.24777546820161142</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.54394312462409933</v>
       </c>
       <c r="C196" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A196^2+B196^2, 0)  + _c2*BESSELJ(_c3*A196^2+_c4*B196^2, 0)  - _c5*BESSELJ(_c6*A196^2+_c7*B196^2, 0)</f>
-        <v>2.9797263417121154</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>-1.627625092009179</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A197">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.33163803779177725</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-0.79136038432004674</v>
       </c>
       <c r="B197">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.29438571979355038</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-0.50554015720008516</v>
       </c>
       <c r="C197" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A197^2+B197^2, 0)  + _c2*BESSELJ(_c3*A197^2+_c4*B197^2, 0)  - _c5*BESSELJ(_c6*A197^2+_c7*B197^2, 0)</f>
-        <v>2.2800181275593339</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>-0.41538901881429879</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A198">
-        <f t="shared" ca="1" si="9"/>
-        <v>-0.18150482429000891</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-0.42424392502451058</v>
       </c>
       <c r="B198">
-        <f t="shared" ca="1" si="9"/>
-        <v>9.7945627194354942E-2</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.14549587881224435</v>
       </c>
       <c r="C198" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A198^2+B198^2, 0)  + _c2*BESSELJ(_c3*A198^2+_c4*B198^2, 0)  - _c5*BESSELJ(_c6*A198^2+_c7*B198^2, 0)</f>
-        <v>3.0115119552020024</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>3.5616731413194915</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A199">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.77720704033197663</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>0.47966127953673982</v>
       </c>
       <c r="B199">
-        <f t="shared" ca="1" si="9"/>
-        <v>6.4355972245997345E-2</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-1.0426962245765155</v>
       </c>
       <c r="C199" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A199^2+B199^2, 0)  + _c2*BESSELJ(_c3*A199^2+_c4*B199^2, 0)  - _c5*BESSELJ(_c6*A199^2+_c7*B199^2, 0)</f>
-        <v>0.47122642376986962</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>0.58320265794243475</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A200">
-        <f t="shared" ca="1" si="9"/>
-        <v>-1.8026223854795482E-2</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-1.2147572244888367E-2</v>
       </c>
       <c r="B200">
-        <f t="shared" ca="1" si="9"/>
-        <v>-0.24975178275431445</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>8.7311204326851757E-2</v>
       </c>
       <c r="C200" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A200^2+B200^2, 0)  + _c2*BESSELJ(_c3*A200^2+_c4*B200^2, 0)  - _c5*BESSELJ(_c6*A200^2+_c7*B200^2, 0)</f>
-        <v>2.6358364506934508</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>2.9943816960746448</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A201">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.10432759806807165</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-0.63256342685527589</v>
       </c>
       <c r="B201">
-        <f t="shared" ca="1" si="9"/>
-        <v>-0.91243413778413607</v>
+        <f t="shared" ca="1" si="12"/>
+        <v>-1.1163464712027544</v>
       </c>
       <c r="C201" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A201^2+B201^2, 0)  + _c2*BESSELJ(_c3*A201^2+_c4*B201^2, 0)  - _c5*BESSELJ(_c6*A201^2+_c7*B201^2, 0)</f>
-        <v>1.3398258744305802</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>0.62413557478709092</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A202">
-        <f t="shared" ref="A202:B225" ca="1" si="10">_xlfn.NORM.INV(RAND(),0,0.5)</f>
-        <v>0.45713079033195625</v>
+        <f t="shared" ref="A202:B225" ca="1" si="14">_xlfn.NORM.INV(RAND(),0,0.5)</f>
+        <v>0.77038505701156668</v>
       </c>
       <c r="B202">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.18205190449106834</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-8.8148281779595966E-2</v>
       </c>
       <c r="C202" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A202^2+B202^2, 0)  + _c2*BESSELJ(_c3*A202^2+_c4*B202^2, 0)  - _c5*BESSELJ(_c6*A202^2+_c7*B202^2, 0)</f>
-        <v>3.5016989359087218</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>0.53748305798295148</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A203">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.80235525829427112</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.33967161724902378</v>
       </c>
       <c r="B203">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.35355117124710489</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.16680607974426967</v>
       </c>
       <c r="C203" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A203^2+B203^2, 0)  + _c2*BESSELJ(_c3*A203^2+_c4*B203^2, 0)  - _c5*BESSELJ(_c6*A203^2+_c7*B203^2, 0)</f>
-        <v>-1.3411892096256199</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>3.1612807307403985</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A204">
-        <f t="shared" ca="1" si="10"/>
-        <v>-4.3861265334686941E-2</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.42689406159844873</v>
       </c>
       <c r="B204">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.76560937081794467</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.43308085072273261</v>
       </c>
       <c r="C204" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A204^2+B204^2, 0)  + _c2*BESSELJ(_c3*A204^2+_c4*B204^2, 0)  - _c5*BESSELJ(_c6*A204^2+_c7*B204^2, 0)</f>
-        <v>0.66104288458491045</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>0.54973351687272554</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A205">
-        <f t="shared" ca="1" si="10"/>
-        <v>-1.0296856448267744</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.77338630388591112</v>
       </c>
       <c r="B205">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.22291810195228856</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.43917277710976338</v>
       </c>
       <c r="C205" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A205^2+B205^2, 0)  + _c2*BESSELJ(_c3*A205^2+_c4*B205^2, 0)  - _c5*BESSELJ(_c6*A205^2+_c7*B205^2, 0)</f>
-        <v>0.10025572113560755</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>-1.1171545182356564</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A206">
-        <f t="shared" ca="1" si="10"/>
-        <v>-8.2641408516000103E-2</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.49681079129841133</v>
       </c>
       <c r="B206">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.75677129939794285</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-8.3273778524217065E-2</v>
       </c>
       <c r="C206" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A206^2+B206^2, 0)  + _c2*BESSELJ(_c3*A206^2+_c4*B206^2, 0)  - _c5*BESSELJ(_c6*A206^2+_c7*B206^2, 0)</f>
-        <v>0.53142425627848766</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>4.0288480717955615</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A207">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.46502919984578162</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.22175250137502345</v>
       </c>
       <c r="B207">
-        <f t="shared" ca="1" si="10"/>
-        <v>9.8702296767747971E-3</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.19953972115030486</v>
       </c>
       <c r="C207" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A207^2+B207^2, 0)  + _c2*BESSELJ(_c3*A207^2+_c4*B207^2, 0)  - _c5*BESSELJ(_c6*A207^2+_c7*B207^2, 0)</f>
-        <v>4.0105685874545554</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>2.8343757751367553</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A208">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.1797853124877401</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.33196344144053652</v>
       </c>
       <c r="B208">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.22742278733933624</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>1.0037010103044923</v>
       </c>
       <c r="C208" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A208^2+B208^2, 0)  + _c2*BESSELJ(_c3*A208^2+_c4*B208^2, 0)  - _c5*BESSELJ(_c6*A208^2+_c7*B208^2, 0)</f>
-        <v>2.7038648059395318</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>0.54162759702270302</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A209">
-        <f t="shared" ca="1" si="10"/>
-        <v>-9.1549093368192225E-2</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>4.4759272334726201E-2</v>
       </c>
       <c r="B209">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.76729899279189118</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.66012880135248275</v>
       </c>
       <c r="C209" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A209^2+B209^2, 0)  + _c2*BESSELJ(_c3*A209^2+_c4*B209^2, 0)  - _c5*BESSELJ(_c6*A209^2+_c7*B209^2, 0)</f>
-        <v>0.80386978121816988</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>-1.6549367378467272</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A210">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.14667143452273246</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>1.8373414065461904E-2</v>
       </c>
       <c r="B210">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.43748668893031267</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.46053982174671976</v>
       </c>
       <c r="C210" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A210^2+B210^2, 0)  + _c2*BESSELJ(_c3*A210^2+_c4*B210^2, 0)  - _c5*BESSELJ(_c6*A210^2+_c7*B210^2, 0)</f>
-        <v>0.18385469658959308</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>-0.19603828897721698</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A211">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.31601057726058324</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>2.3579439406020124E-2</v>
       </c>
       <c r="B211">
-        <f t="shared" ca="1" si="10"/>
-        <v>6.4351375280872536E-2</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-3.1366221580164111E-2</v>
       </c>
       <c r="C211" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A211^2+B211^2, 0)  + _c2*BESSELJ(_c3*A211^2+_c4*B211^2, 0)  - _c5*BESSELJ(_c6*A211^2+_c7*B211^2, 0)</f>
-        <v>3.284656261093188</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>2.9998901385167263</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A212">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.92076902998958277</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-1.2347621702147333</v>
       </c>
       <c r="B212">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.46621490353893752</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.43657857041578368</v>
       </c>
       <c r="C212" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A212^2+B212^2, 0)  + _c2*BESSELJ(_c3*A212^2+_c4*B212^2, 0)  - _c5*BESSELJ(_c6*A212^2+_c7*B212^2, 0)</f>
-        <v>1.0388811489158631</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>1.382624096038779</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A213">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.54047634570706049</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>1.0296010100689685</v>
       </c>
       <c r="B213">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.7218773405039095</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>7.7786659482313308E-2</v>
       </c>
       <c r="C213" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A213^2+B213^2, 0)  + _c2*BESSELJ(_c3*A213^2+_c4*B213^2, 0)  - _c5*BESSELJ(_c6*A213^2+_c7*B213^2, 0)</f>
-        <v>2.447716012211107</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>-0.25671859187483598</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A214">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.37732725706991332</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.33251521714127941</v>
       </c>
       <c r="B214">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.71634278335847879</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.7908314327884709</v>
       </c>
       <c r="C214" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A214^2+B214^2, 0)  + _c2*BESSELJ(_c3*A214^2+_c4*B214^2, 0)  - _c5*BESSELJ(_c6*A214^2+_c7*B214^2, 0)</f>
-        <v>1.6310117833783411</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>2.5156936618854475</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A215">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.29997096884358887</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.60070369302293691</v>
       </c>
       <c r="B215">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.11467466609037047</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.67080983187342591</v>
       </c>
       <c r="C215" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A215^2+B215^2, 0)  + _c2*BESSELJ(_c3*A215^2+_c4*B215^2, 0)  - _c5*BESSELJ(_c6*A215^2+_c7*B215^2, 0)</f>
-        <v>3.1768420127124699</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>1.7630335402236041</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A216">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.30488271277148421</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.11715889086660028</v>
       </c>
       <c r="B216">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.26494285218016844</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.17265382360286941</v>
       </c>
       <c r="C216" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A216^2+B216^2, 0)  + _c2*BESSELJ(_c3*A216^2+_c4*B216^2, 0)  - _c5*BESSELJ(_c6*A216^2+_c7*B216^2, 0)</f>
-        <v>2.5198649864690168</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>2.9014973410435299</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A217">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.18839828417202695</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.37360015380464179</v>
       </c>
       <c r="B217">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.73968975448805629</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.81907028576384322</v>
       </c>
       <c r="C217" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A217^2+B217^2, 0)  + _c2*BESSELJ(_c3*A217^2+_c4*B217^2, 0)  - _c5*BESSELJ(_c6*A217^2+_c7*B217^2, 0)</f>
-        <v>0.59069124252308403</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>2.7371239947853421</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A218">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.13778216467331547</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>3.8314352155270062E-3</v>
       </c>
       <c r="B218">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.18390156167038649</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>2.2946062463049557E-2</v>
       </c>
       <c r="C218" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A218^2+B218^2, 0)  + _c2*BESSELJ(_c3*A218^2+_c4*B218^2, 0)  - _c5*BESSELJ(_c6*A218^2+_c7*B218^2, 0)</f>
-        <v>2.8718291031062182</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>2.9999730811752938</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A219">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.62585511978685948</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-5.9020040093392824E-2</v>
       </c>
       <c r="B219">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.23489064052447148</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.65416377176554052</v>
       </c>
       <c r="C219" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A219^2+B219^2, 0)  + _c2*BESSELJ(_c3*A219^2+_c4*B219^2, 0)  - _c5*BESSELJ(_c6*A219^2+_c7*B219^2, 0)</f>
-        <v>2.3559594152183148</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>-1.7153092169436563</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A220">
-        <f t="shared" ca="1" si="10"/>
-        <v>-1.6325427668241006</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.2078112726515523</v>
       </c>
       <c r="B220">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.81793306172052616</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>5.6004715798890006E-2</v>
       </c>
       <c r="C220" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A220^2+B220^2, 0)  + _c2*BESSELJ(_c3*A220^2+_c4*B220^2, 0)  - _c5*BESSELJ(_c6*A220^2+_c7*B220^2, 0)</f>
-        <v>-0.58301981765670119</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>3.0540910819257219</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A221">
-        <f t="shared" ca="1" si="10"/>
-        <v>-3.3760597363699532E-2</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.5439717273826612</v>
       </c>
       <c r="B221">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.24386137962121876</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.18688692587340497</v>
       </c>
       <c r="C221" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A221^2+B221^2, 0)  + _c2*BESSELJ(_c3*A221^2+_c4*B221^2, 0)  - _c5*BESSELJ(_c6*A221^2+_c7*B221^2, 0)</f>
-        <v>2.6659411972846012</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>3.5082986704692773</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A222">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.7744188149665846</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-0.31037517974554385</v>
       </c>
       <c r="B222">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.16769961430622582</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.7325728017054578</v>
       </c>
       <c r="C222" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A222^2+B222^2, 0)  + _c2*BESSELJ(_c3*A222^2+_c4*B222^2, 0)  - _c5*BESSELJ(_c6*A222^2+_c7*B222^2, 0)</f>
-        <v>2.4294481880264618E-2</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>1.376990605642983</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A223">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.21337943450663699</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>-8.2639348277518773E-2</v>
       </c>
       <c r="B223">
-        <f t="shared" ca="1" si="10"/>
-        <v>-6.2010493414477827E-2</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>5.1588161061326361E-2</v>
       </c>
       <c r="C223" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A223^2+B223^2, 0)  + _c2*BESSELJ(_c3*A223^2+_c4*B223^2, 0)  - _c5*BESSELJ(_c6*A223^2+_c7*B223^2, 0)</f>
-        <v>3.0583806607976332</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>2.999977532788666</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A224">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.54402576573971861</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.4899265913188654</v>
       </c>
       <c r="B224">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.44741312922487858</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>1.0690784785652365</v>
       </c>
       <c r="C224" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A224^2+B224^2, 0)  + _c2*BESSELJ(_c3*A224^2+_c4*B224^2, 0)  - _c5*BESSELJ(_c6*A224^2+_c7*B224^2, 0)</f>
-        <v>0.4490944432246653</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>0.885253650587428</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A225">
-        <f t="shared" ca="1" si="10"/>
-        <v>0.43274859672641269</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.81101185722845326</v>
       </c>
       <c r="B225">
-        <f t="shared" ca="1" si="10"/>
-        <v>-0.16661157408464594</v>
+        <f t="shared" ca="1" si="14"/>
+        <v>0.10507827603887493</v>
       </c>
       <c r="C225" s="1">
-        <f ca="1" xml:space="preserve"> _c1*BESSELJ(A225^2+B225^2, 0)  + _c2*BESSELJ(_c3*A225^2+_c4*B225^2, 0)  - _c5*BESSELJ(_c6*A225^2+_c7*B225^2, 0)</f>
-        <v>3.5031880286998867</v>
+        <f t="shared" ca="1" si="13"/>
+        <v>-0.30123844541056244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>